<commit_message>
Update database and start to add achievement, now having Tralfagar D. Law trophies and personal award
</commit_message>
<xml_diff>
--- a/player_info.xlsx
+++ b/player_info.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="310">
   <si>
     <t>name</t>
   </si>
@@ -527,6 +527,15 @@
   </si>
   <si>
     <t>1900-9-5</t>
+  </si>
+  <si>
+    <t>Elfman Strauss</t>
+  </si>
+  <si>
+    <t>ft_5</t>
+  </si>
+  <si>
+    <t>1900-8-2</t>
   </si>
   <si>
     <t>Hisoka Morow</t>
@@ -2097,7 +2106,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G100"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A2" xSplit="0" ySplit="1" activePane="bottomLeft" state="frozen"/>
@@ -3368,7 +3377,7 @@
         <v>11</v>
       </c>
       <c r="F55" s="6">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="G55" t="s" s="5">
         <v>12</v>
@@ -3382,7 +3391,7 @@
         <v>176</v>
       </c>
       <c r="C56" t="s" s="5">
-        <v>139</v>
+        <v>177</v>
       </c>
       <c r="D56" t="s" s="5">
         <v>10</v>
@@ -3391,7 +3400,7 @@
         <v>11</v>
       </c>
       <c r="F56" s="6">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G56" t="s" s="5">
         <v>12</v>
@@ -3399,13 +3408,13 @@
     </row>
     <row r="57" ht="50.35" customHeight="1">
       <c r="A57" t="s" s="5">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B57" t="s" s="5">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C57" t="s" s="5">
-        <v>179</v>
+        <v>139</v>
       </c>
       <c r="D57" t="s" s="5">
         <v>10</v>
@@ -3414,7 +3423,7 @@
         <v>11</v>
       </c>
       <c r="F57" s="6">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="G57" t="s" s="5">
         <v>12</v>
@@ -3437,7 +3446,7 @@
         <v>11</v>
       </c>
       <c r="F58" s="6">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="G58" t="s" s="5">
         <v>12</v>
@@ -3460,7 +3469,7 @@
         <v>11</v>
       </c>
       <c r="F59" s="6">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G59" t="s" s="5">
         <v>12</v>
@@ -3483,7 +3492,7 @@
         <v>11</v>
       </c>
       <c r="F60" s="6">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="G60" t="s" s="5">
         <v>12</v>
@@ -3529,7 +3538,7 @@
         <v>11</v>
       </c>
       <c r="F62" s="6">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="G62" t="s" s="5">
         <v>12</v>
@@ -3552,7 +3561,7 @@
         <v>11</v>
       </c>
       <c r="F63" s="6">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="G63" t="s" s="5">
         <v>12</v>
@@ -3575,7 +3584,7 @@
         <v>11</v>
       </c>
       <c r="F64" s="6">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G64" t="s" s="5">
         <v>12</v>
@@ -3598,7 +3607,7 @@
         <v>11</v>
       </c>
       <c r="F65" s="6">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="G65" t="s" s="5">
         <v>12</v>
@@ -3615,13 +3624,13 @@
         <v>206</v>
       </c>
       <c r="D66" t="s" s="5">
-        <v>207</v>
+        <v>10</v>
       </c>
       <c r="E66" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F66" s="6">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="G66" t="s" s="5">
         <v>12</v>
@@ -3629,22 +3638,22 @@
     </row>
     <row r="67" ht="50.35" customHeight="1">
       <c r="A67" t="s" s="5">
+        <v>207</v>
+      </c>
+      <c r="B67" t="s" s="5">
         <v>208</v>
       </c>
-      <c r="B67" t="s" s="5">
+      <c r="C67" t="s" s="5">
         <v>209</v>
       </c>
-      <c r="C67" t="s" s="5">
+      <c r="D67" t="s" s="5">
         <v>210</v>
       </c>
-      <c r="D67" t="s" s="5">
-        <v>211</v>
-      </c>
       <c r="E67" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F67" s="6">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G67" t="s" s="5">
         <v>12</v>
@@ -3652,22 +3661,22 @@
     </row>
     <row r="68" ht="50.35" customHeight="1">
       <c r="A68" t="s" s="5">
+        <v>211</v>
+      </c>
+      <c r="B68" t="s" s="5">
         <v>212</v>
       </c>
-      <c r="B68" t="s" s="5">
+      <c r="C68" t="s" s="5">
         <v>213</v>
       </c>
-      <c r="C68" t="s" s="5">
-        <v>76</v>
-      </c>
       <c r="D68" t="s" s="5">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E68" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F68" s="6">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="G68" t="s" s="5">
         <v>12</v>
@@ -3675,22 +3684,22 @@
     </row>
     <row r="69" ht="50.35" customHeight="1">
       <c r="A69" t="s" s="5">
+        <v>215</v>
+      </c>
+      <c r="B69" t="s" s="5">
+        <v>216</v>
+      </c>
+      <c r="C69" t="s" s="5">
+        <v>76</v>
+      </c>
+      <c r="D69" t="s" s="5">
         <v>214</v>
       </c>
-      <c r="B69" t="s" s="5">
-        <v>215</v>
-      </c>
-      <c r="C69" t="s" s="5">
-        <v>216</v>
-      </c>
-      <c r="D69" t="s" s="5">
-        <v>217</v>
-      </c>
       <c r="E69" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F69" s="6">
-        <v>240</v>
+        <v>167</v>
       </c>
       <c r="G69" t="s" s="5">
         <v>12</v>
@@ -3698,22 +3707,22 @@
     </row>
     <row r="70" ht="50.35" customHeight="1">
       <c r="A70" t="s" s="5">
+        <v>217</v>
+      </c>
+      <c r="B70" t="s" s="5">
         <v>218</v>
       </c>
-      <c r="B70" t="s" s="5">
+      <c r="C70" t="s" s="5">
         <v>219</v>
       </c>
-      <c r="C70" t="s" s="5">
-        <v>185</v>
-      </c>
       <c r="D70" t="s" s="5">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="E70" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F70" s="6">
-        <v>174</v>
+        <v>240</v>
       </c>
       <c r="G70" t="s" s="5">
         <v>12</v>
@@ -3721,22 +3730,22 @@
     </row>
     <row r="71" ht="50.35" customHeight="1">
       <c r="A71" t="s" s="5">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B71" t="s" s="5">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C71" t="s" s="5">
-        <v>222</v>
+        <v>188</v>
       </c>
       <c r="D71" t="s" s="5">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E71" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F71" s="6">
-        <v>201</v>
+        <v>174</v>
       </c>
       <c r="G71" t="s" s="5">
         <v>12</v>
@@ -3744,22 +3753,22 @@
     </row>
     <row r="72" ht="50.35" customHeight="1">
       <c r="A72" t="s" s="5">
+        <v>223</v>
+      </c>
+      <c r="B72" t="s" s="5">
         <v>224</v>
       </c>
-      <c r="B72" t="s" s="5">
+      <c r="C72" t="s" s="5">
         <v>225</v>
       </c>
-      <c r="C72" t="s" s="5">
+      <c r="D72" t="s" s="5">
         <v>226</v>
       </c>
-      <c r="D72" t="s" s="5">
-        <v>227</v>
-      </c>
       <c r="E72" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F72" s="6">
-        <v>180</v>
+        <v>201</v>
       </c>
       <c r="G72" t="s" s="5">
         <v>12</v>
@@ -3767,22 +3776,22 @@
     </row>
     <row r="73" ht="50.35" customHeight="1">
       <c r="A73" t="s" s="5">
+        <v>227</v>
+      </c>
+      <c r="B73" t="s" s="5">
         <v>228</v>
       </c>
-      <c r="B73" t="s" s="5">
+      <c r="C73" t="s" s="5">
         <v>229</v>
       </c>
-      <c r="C73" t="s" s="5">
+      <c r="D73" t="s" s="5">
         <v>230</v>
       </c>
-      <c r="D73" t="s" s="5">
-        <v>227</v>
-      </c>
       <c r="E73" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F73" s="6">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="G73" t="s" s="5">
         <v>12</v>
@@ -3799,13 +3808,13 @@
         <v>233</v>
       </c>
       <c r="D74" t="s" s="5">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E74" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F74" s="6">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="G74" t="s" s="5">
         <v>12</v>
@@ -3822,13 +3831,13 @@
         <v>236</v>
       </c>
       <c r="D75" t="s" s="5">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E75" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F75" s="6">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="G75" t="s" s="5">
         <v>12</v>
@@ -3845,13 +3854,13 @@
         <v>239</v>
       </c>
       <c r="D76" t="s" s="5">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E76" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F76" s="6">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="G76" t="s" s="5">
         <v>12</v>
@@ -3868,13 +3877,13 @@
         <v>242</v>
       </c>
       <c r="D77" t="s" s="5">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="E77" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F77" s="6">
-        <v>150</v>
+        <v>190</v>
       </c>
       <c r="G77" t="s" s="5">
         <v>12</v>
@@ -3882,22 +3891,22 @@
     </row>
     <row r="78" ht="50.35" customHeight="1">
       <c r="A78" t="s" s="5">
+        <v>243</v>
+      </c>
+      <c r="B78" t="s" s="5">
         <v>244</v>
       </c>
-      <c r="B78" t="s" s="5">
+      <c r="C78" t="s" s="5">
         <v>245</v>
       </c>
-      <c r="C78" t="s" s="5">
-        <v>50</v>
-      </c>
       <c r="D78" t="s" s="5">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="E78" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F78" s="6">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="G78" t="s" s="5">
         <v>12</v>
@@ -3905,22 +3914,22 @@
     </row>
     <row r="79" ht="50.35" customHeight="1">
       <c r="A79" t="s" s="5">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B79" t="s" s="5">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C79" t="s" s="5">
-        <v>248</v>
+        <v>50</v>
       </c>
       <c r="D79" t="s" s="5">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="E79" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F79" s="6">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="G79" t="s" s="5">
         <v>12</v>
@@ -3937,7 +3946,7 @@
         <v>251</v>
       </c>
       <c r="D80" t="s" s="5">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="E80" t="s" s="5">
         <v>11</v>
@@ -3960,13 +3969,13 @@
         <v>254</v>
       </c>
       <c r="D81" t="s" s="5">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="E81" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F81" s="6">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="G81" t="s" s="5">
         <v>12</v>
@@ -3974,22 +3983,22 @@
     </row>
     <row r="82" ht="50.35" customHeight="1">
       <c r="A82" t="s" s="5">
+        <v>255</v>
+      </c>
+      <c r="B82" t="s" s="5">
         <v>256</v>
       </c>
-      <c r="B82" t="s" s="5">
+      <c r="C82" t="s" s="5">
         <v>257</v>
       </c>
-      <c r="C82" t="s" s="5">
+      <c r="D82" t="s" s="5">
         <v>258</v>
       </c>
-      <c r="D82" t="s" s="5">
-        <v>223</v>
-      </c>
       <c r="E82" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F82" s="6">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="G82" t="s" s="5">
         <v>12</v>
@@ -4006,13 +4015,13 @@
         <v>261</v>
       </c>
       <c r="D83" t="s" s="5">
-        <v>207</v>
+        <v>226</v>
       </c>
       <c r="E83" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F83" s="6">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="G83" t="s" s="5">
         <v>12</v>
@@ -4029,13 +4038,13 @@
         <v>264</v>
       </c>
       <c r="D84" t="s" s="5">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="E84" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F84" s="6">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="G84" t="s" s="5">
         <v>12</v>
@@ -4052,13 +4061,13 @@
         <v>267</v>
       </c>
       <c r="D85" t="s" s="5">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="E85" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F85" s="6">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G85" t="s" s="5">
         <v>12</v>
@@ -4075,13 +4084,13 @@
         <v>270</v>
       </c>
       <c r="D86" t="s" s="5">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E86" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F86" s="6">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="G86" t="s" s="5">
         <v>12</v>
@@ -4098,13 +4107,13 @@
         <v>273</v>
       </c>
       <c r="D87" t="s" s="5">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E87" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F87" s="6">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="G87" t="s" s="5">
         <v>12</v>
@@ -4121,13 +4130,13 @@
         <v>276</v>
       </c>
       <c r="D88" t="s" s="5">
-        <v>10</v>
+        <v>220</v>
       </c>
       <c r="E88" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F88" s="6">
-        <v>175</v>
+        <v>219</v>
       </c>
       <c r="G88" t="s" s="5">
         <v>12</v>
@@ -4150,7 +4159,7 @@
         <v>11</v>
       </c>
       <c r="F89" s="6">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="G89" t="s" s="5">
         <v>12</v>
@@ -4173,7 +4182,7 @@
         <v>11</v>
       </c>
       <c r="F90" s="6">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="G90" t="s" s="5">
         <v>12</v>
@@ -4196,7 +4205,7 @@
         <v>11</v>
       </c>
       <c r="F91" s="6">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="G91" t="s" s="5">
         <v>12</v>
@@ -4219,7 +4228,7 @@
         <v>11</v>
       </c>
       <c r="F92" s="6">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="G92" t="s" s="5">
         <v>12</v>
@@ -4242,7 +4251,7 @@
         <v>11</v>
       </c>
       <c r="F93" s="6">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="G93" t="s" s="5">
         <v>12</v>
@@ -4259,13 +4268,13 @@
         <v>294</v>
       </c>
       <c r="D94" t="s" s="5">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="E94" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F94" s="6">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="G94" t="s" s="5">
         <v>12</v>
@@ -4302,7 +4311,7 @@
         <v>299</v>
       </c>
       <c r="C96" t="s" s="5">
-        <v>188</v>
+        <v>300</v>
       </c>
       <c r="D96" t="s" s="5">
         <v>41</v>
@@ -4319,13 +4328,13 @@
     </row>
     <row r="97" ht="50.35" customHeight="1">
       <c r="A97" t="s" s="5">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B97" t="s" s="5">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C97" t="s" s="5">
-        <v>102</v>
+        <v>191</v>
       </c>
       <c r="D97" t="s" s="5">
         <v>41</v>
@@ -4334,7 +4343,7 @@
         <v>11</v>
       </c>
       <c r="F97" s="6">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G97" t="s" s="5">
         <v>12</v>
@@ -4342,13 +4351,13 @@
     </row>
     <row r="98" ht="50.35" customHeight="1">
       <c r="A98" t="s" s="5">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B98" t="s" s="5">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C98" t="s" s="5">
-        <v>304</v>
+        <v>102</v>
       </c>
       <c r="D98" t="s" s="5">
         <v>41</v>
@@ -4357,7 +4366,7 @@
         <v>11</v>
       </c>
       <c r="F98" s="6">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="G98" t="s" s="5">
         <v>12</v>
@@ -4371,7 +4380,7 @@
         <v>306</v>
       </c>
       <c r="C99" t="s" s="5">
-        <v>216</v>
+        <v>307</v>
       </c>
       <c r="D99" t="s" s="5">
         <v>41</v>
@@ -4380,20 +4389,43 @@
         <v>11</v>
       </c>
       <c r="F99" s="6">
+        <v>180</v>
+      </c>
+      <c r="G99" t="s" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" ht="50.35" customHeight="1">
+      <c r="A100" t="s" s="5">
+        <v>308</v>
+      </c>
+      <c r="B100" t="s" s="5">
+        <v>309</v>
+      </c>
+      <c r="C100" t="s" s="5">
+        <v>219</v>
+      </c>
+      <c r="D100" t="s" s="5">
+        <v>41</v>
+      </c>
+      <c r="E100" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F100" s="6">
         <v>175</v>
       </c>
-      <c r="G99" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="100" ht="20.05" customHeight="1">
-      <c r="A100" s="7"/>
-      <c r="B100" s="7"/>
-      <c r="C100" s="7"/>
-      <c r="D100" s="7"/>
-      <c r="E100" s="7"/>
-      <c r="F100" s="7"/>
-      <c r="G100" s="7"/>
+      <c r="G100" t="s" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" ht="20.05" customHeight="1">
+      <c r="A101" s="7"/>
+      <c r="B101" s="7"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="7"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="7"/>
+      <c r="G101" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>

<commit_message>
Update the Frontpage and the database.
</commit_message>
<xml_diff>
--- a/player_info.xlsx
+++ b/player_info.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="313">
   <si>
     <t>name</t>
   </si>
@@ -34,6 +34,24 @@
     <t>biography</t>
   </si>
   <si>
+    <t>Kiyotaka Ayanokouji</t>
+  </si>
+  <si>
+    <t>cote_10</t>
+  </si>
+  <si>
+    <t>1900-10-20</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Genius of White Room, Mastermind of everywhere he goes, great tactician, but little who know he really is.; Good skills for playing football, can evaluate and analyse what happened in the pitch, but only keeps in his mind while he is playing, need to be understood or his team will lose because of disconnection.</t>
+  </si>
+  <si>
     <t>Manabu Horikita</t>
   </si>
   <si>
@@ -43,12 +61,6 @@
     <t>1900-4-24</t>
   </si>
   <si>
-    <t>Japan</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
     <t>Loading biography......</t>
   </si>
   <si>
@@ -56,9 +68,6 @@
   </si>
   <si>
     <t>cote_25</t>
-  </si>
-  <si>
-    <t>1900-10-20</t>
   </si>
   <si>
     <t>Yosuke Hirata</t>
@@ -2106,7 +2115,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A2" xSplit="0" ySplit="1" activePane="bottomLeft" state="frozen"/>
@@ -2114,7 +2123,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.2734" style="1" customWidth="1"/>
+    <col min="2" max="6" width="16.3516" style="1" customWidth="1"/>
+    <col min="7" max="7" width="96.6406" style="1" customWidth="1"/>
     <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2141,7 +2152,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="50.55" customHeight="1">
+    <row r="2" ht="82.55" customHeight="1">
       <c r="A2" t="s" s="3">
         <v>7</v>
       </c>
@@ -2158,13 +2169,13 @@
         <v>11</v>
       </c>
       <c r="F2" s="4">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G2" t="s" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="3" ht="50.35" customHeight="1">
+    <row r="3" ht="18.35" customHeight="1">
       <c r="A3" t="s" s="5">
         <v>13</v>
       </c>
@@ -2181,21 +2192,21 @@
         <v>11</v>
       </c>
       <c r="F3" s="6">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G3" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" ht="18.35" customHeight="1">
       <c r="A4" t="s" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s" s="5">
         <v>10</v>
@@ -2207,10 +2218,10 @@
         <v>174</v>
       </c>
       <c r="G4" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" ht="18.35" customHeight="1">
       <c r="A5" t="s" s="5">
         <v>19</v>
       </c>
@@ -2221,65 +2232,65 @@
         <v>21</v>
       </c>
       <c r="D5" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F5" s="6">
+        <v>174</v>
+      </c>
+      <c r="G5" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" ht="18.35" customHeight="1">
+      <c r="A6" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="E5" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F5" s="6">
+      <c r="B6" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s" s="5">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F6" s="6">
         <v>183</v>
       </c>
-      <c r="G5" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" ht="50.35" customHeight="1">
-      <c r="A6" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s" s="5">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s" s="5">
+      <c r="G6" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" ht="34.35" customHeight="1">
+      <c r="A7" t="s" s="5">
         <v>26</v>
       </c>
-      <c r="E6" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="B7" t="s" s="5">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s" s="5">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s" s="5">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F7" s="6">
         <v>160</v>
       </c>
-      <c r="G6" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" ht="50.35" customHeight="1">
-      <c r="A7" t="s" s="5">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s" s="5">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s" s="5">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F7" s="6">
-        <v>169</v>
-      </c>
       <c r="G7" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" ht="18.35" customHeight="1">
       <c r="A8" t="s" s="5">
         <v>30</v>
       </c>
@@ -2290,88 +2301,88 @@
         <v>32</v>
       </c>
       <c r="D8" t="s" s="5">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F8" s="6">
+        <v>169</v>
+      </c>
+      <c r="G8" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" ht="18.35" customHeight="1">
+      <c r="A9" t="s" s="5">
         <v>33</v>
       </c>
-      <c r="E8" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F8" s="6">
+      <c r="B9" t="s" s="5">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s" s="5">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s" s="5">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F9" s="6">
         <v>183</v>
       </c>
-      <c r="G8" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" ht="50.35" customHeight="1">
-      <c r="A9" t="s" s="5">
-        <v>34</v>
-      </c>
-      <c r="B9" t="s" s="5">
-        <v>35</v>
-      </c>
-      <c r="C9" t="s" s="5">
-        <v>36</v>
-      </c>
-      <c r="D9" t="s" s="5">
+      <c r="G9" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" ht="18.35" customHeight="1">
+      <c r="A10" t="s" s="5">
         <v>37</v>
       </c>
-      <c r="E9" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F9" s="6">
+      <c r="B10" t="s" s="5">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s" s="5">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s" s="5">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F10" s="6">
         <v>175</v>
       </c>
-      <c r="G9" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" ht="50.35" customHeight="1">
-      <c r="A10" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="B10" t="s" s="5">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s" s="5">
-        <v>40</v>
-      </c>
-      <c r="D10" t="s" s="5">
+      <c r="G10" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" ht="18.35" customHeight="1">
+      <c r="A11" t="s" s="5">
         <v>41</v>
       </c>
-      <c r="E10" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F10" s="6">
+      <c r="B11" t="s" s="5">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s" s="5">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s" s="5">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F11" s="6">
         <v>163</v>
       </c>
-      <c r="G10" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" ht="50.35" customHeight="1">
-      <c r="A11" t="s" s="5">
-        <v>42</v>
-      </c>
-      <c r="B11" t="s" s="5">
-        <v>43</v>
-      </c>
-      <c r="C11" t="s" s="5">
-        <v>44</v>
-      </c>
-      <c r="D11" t="s" s="5">
-        <v>41</v>
-      </c>
-      <c r="E11" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F11" s="6">
-        <v>170</v>
-      </c>
       <c r="G11" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" ht="18.35" customHeight="1">
       <c r="A12" t="s" s="5">
         <v>45</v>
       </c>
@@ -2382,19 +2393,19 @@
         <v>47</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F12" s="6">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="G12" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" ht="18.35" customHeight="1">
       <c r="A13" t="s" s="5">
         <v>48</v>
       </c>
@@ -2405,19 +2416,19 @@
         <v>50</v>
       </c>
       <c r="D13" t="s" s="5">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F13" s="6">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="G13" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" ht="18.35" customHeight="1">
       <c r="A14" t="s" s="5">
         <v>51</v>
       </c>
@@ -2428,19 +2439,19 @@
         <v>53</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F14" s="6">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="G14" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" ht="18.35" customHeight="1">
       <c r="A15" t="s" s="5">
         <v>54</v>
       </c>
@@ -2451,53 +2462,53 @@
         <v>56</v>
       </c>
       <c r="D15" t="s" s="5">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F15" s="6">
+        <v>155</v>
+      </c>
+      <c r="G15" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" ht="18.35" customHeight="1">
+      <c r="A16" t="s" s="5">
         <v>57</v>
       </c>
-      <c r="E15" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F15" s="6">
+      <c r="B16" t="s" s="5">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s" s="5">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s" s="5">
+        <v>60</v>
+      </c>
+      <c r="E16" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F16" s="6">
         <v>172</v>
       </c>
-      <c r="G15" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" ht="50.35" customHeight="1">
-      <c r="A16" t="s" s="5">
-        <v>58</v>
-      </c>
-      <c r="B16" t="s" s="5">
-        <v>59</v>
-      </c>
-      <c r="C16" t="s" s="5">
-        <v>60</v>
-      </c>
-      <c r="D16" t="s" s="5">
+      <c r="G16" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" ht="18.35" customHeight="1">
+      <c r="A17" t="s" s="5">
         <v>61</v>
       </c>
-      <c r="E16" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F16" s="6">
-        <v>183</v>
-      </c>
-      <c r="G16" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" ht="50.35" customHeight="1">
-      <c r="A17" t="s" s="5">
+      <c r="B17" t="s" s="5">
         <v>62</v>
       </c>
-      <c r="B17" t="s" s="5">
+      <c r="C17" t="s" s="5">
         <v>63</v>
       </c>
-      <c r="C17" t="s" s="5">
+      <c r="D17" t="s" s="5">
         <v>64</v>
-      </c>
-      <c r="D17" t="s" s="5">
-        <v>57</v>
       </c>
       <c r="E17" t="s" s="5">
         <v>11</v>
@@ -2506,10 +2517,10 @@
         <v>183</v>
       </c>
       <c r="G17" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" ht="18.35" customHeight="1">
       <c r="A18" t="s" s="5">
         <v>65</v>
       </c>
@@ -2520,19 +2531,19 @@
         <v>67</v>
       </c>
       <c r="D18" t="s" s="5">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F18" s="6">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="G18" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" ht="18.35" customHeight="1">
       <c r="A19" t="s" s="5">
         <v>68</v>
       </c>
@@ -2543,19 +2554,19 @@
         <v>70</v>
       </c>
       <c r="D19" t="s" s="5">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F19" s="6">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G19" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" ht="18.35" customHeight="1">
       <c r="A20" t="s" s="5">
         <v>71</v>
       </c>
@@ -2566,19 +2577,19 @@
         <v>73</v>
       </c>
       <c r="D20" t="s" s="5">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F20" s="6">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="G20" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" ht="18.35" customHeight="1">
       <c r="A21" t="s" s="5">
         <v>74</v>
       </c>
@@ -2589,19 +2600,19 @@
         <v>76</v>
       </c>
       <c r="D21" t="s" s="5">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F21" s="6">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G21" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" ht="18.35" customHeight="1">
       <c r="A22" t="s" s="5">
         <v>77</v>
       </c>
@@ -2612,19 +2623,19 @@
         <v>79</v>
       </c>
       <c r="D22" t="s" s="5">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E22" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F22" s="6">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G22" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" ht="18.35" customHeight="1">
       <c r="A23" t="s" s="5">
         <v>80</v>
       </c>
@@ -2641,13 +2652,13 @@
         <v>11</v>
       </c>
       <c r="F23" s="6">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G23" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" ht="18.35" customHeight="1">
       <c r="A24" t="s" s="5">
         <v>83</v>
       </c>
@@ -2664,13 +2675,13 @@
         <v>11</v>
       </c>
       <c r="F24" s="6">
-        <v>134</v>
+        <v>180</v>
       </c>
       <c r="G24" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" ht="18.35" customHeight="1">
       <c r="A25" t="s" s="5">
         <v>86</v>
       </c>
@@ -2687,13 +2698,13 @@
         <v>11</v>
       </c>
       <c r="F25" s="6">
-        <v>186</v>
+        <v>134</v>
       </c>
       <c r="G25" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" ht="18.35" customHeight="1">
       <c r="A26" t="s" s="5">
         <v>89</v>
       </c>
@@ -2713,10 +2724,10 @@
         <v>186</v>
       </c>
       <c r="G26" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" ht="34.35" customHeight="1">
       <c r="A27" t="s" s="5">
         <v>92</v>
       </c>
@@ -2724,7 +2735,7 @@
         <v>93</v>
       </c>
       <c r="C27" t="s" s="5">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="D27" t="s" s="5">
         <v>10</v>
@@ -2733,36 +2744,36 @@
         <v>11</v>
       </c>
       <c r="F27" s="6">
+        <v>186</v>
+      </c>
+      <c r="G27" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" ht="18.35" customHeight="1">
+      <c r="A28" t="s" s="5">
+        <v>95</v>
+      </c>
+      <c r="B28" t="s" s="5">
+        <v>96</v>
+      </c>
+      <c r="C28" t="s" s="5">
+        <v>67</v>
+      </c>
+      <c r="D28" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F28" s="6">
         <v>174</v>
       </c>
-      <c r="G27" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" ht="50.35" customHeight="1">
-      <c r="A28" t="s" s="5">
-        <v>94</v>
-      </c>
-      <c r="B28" t="s" s="5">
-        <v>95</v>
-      </c>
-      <c r="C28" t="s" s="5">
-        <v>96</v>
-      </c>
-      <c r="D28" t="s" s="5">
-        <v>10</v>
-      </c>
-      <c r="E28" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F28" s="6">
-        <v>177</v>
-      </c>
       <c r="G28" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" ht="18.35" customHeight="1">
       <c r="A29" t="s" s="5">
         <v>97</v>
       </c>
@@ -2782,10 +2793,10 @@
         <v>177</v>
       </c>
       <c r="G29" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" ht="18.35" customHeight="1">
       <c r="A30" t="s" s="5">
         <v>100</v>
       </c>
@@ -2802,13 +2813,13 @@
         <v>11</v>
       </c>
       <c r="F30" s="6">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G30" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" ht="18.35" customHeight="1">
       <c r="A31" t="s" s="5">
         <v>103</v>
       </c>
@@ -2825,13 +2836,13 @@
         <v>11</v>
       </c>
       <c r="F31" s="6">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G31" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" ht="18.35" customHeight="1">
       <c r="A32" t="s" s="5">
         <v>106</v>
       </c>
@@ -2848,13 +2859,13 @@
         <v>11</v>
       </c>
       <c r="F32" s="6">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="G32" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" ht="18.35" customHeight="1">
       <c r="A33" t="s" s="5">
         <v>109</v>
       </c>
@@ -2871,13 +2882,13 @@
         <v>11</v>
       </c>
       <c r="F33" s="6">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="G33" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" ht="18.35" customHeight="1">
       <c r="A34" t="s" s="5">
         <v>112</v>
       </c>
@@ -2894,13 +2905,13 @@
         <v>11</v>
       </c>
       <c r="F34" s="6">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="G34" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" ht="18.35" customHeight="1">
       <c r="A35" t="s" s="5">
         <v>115</v>
       </c>
@@ -2917,13 +2928,13 @@
         <v>11</v>
       </c>
       <c r="F35" s="6">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="G35" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" ht="18.35" customHeight="1">
       <c r="A36" t="s" s="5">
         <v>118</v>
       </c>
@@ -2931,7 +2942,7 @@
         <v>119</v>
       </c>
       <c r="C36" t="s" s="5">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="D36" t="s" s="5">
         <v>10</v>
@@ -2940,36 +2951,36 @@
         <v>11</v>
       </c>
       <c r="F36" s="6">
+        <v>179</v>
+      </c>
+      <c r="G36" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" ht="18.35" customHeight="1">
+      <c r="A37" t="s" s="5">
+        <v>121</v>
+      </c>
+      <c r="B37" t="s" s="5">
+        <v>122</v>
+      </c>
+      <c r="C37" t="s" s="5">
+        <v>102</v>
+      </c>
+      <c r="D37" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="E37" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F37" s="6">
         <v>165</v>
       </c>
-      <c r="G36" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" ht="50.35" customHeight="1">
-      <c r="A37" t="s" s="5">
-        <v>120</v>
-      </c>
-      <c r="B37" t="s" s="5">
-        <v>121</v>
-      </c>
-      <c r="C37" t="s" s="5">
-        <v>122</v>
-      </c>
-      <c r="D37" t="s" s="5">
-        <v>10</v>
-      </c>
-      <c r="E37" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F37" s="6">
-        <v>198</v>
-      </c>
       <c r="G37" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" ht="18.35" customHeight="1">
       <c r="A38" t="s" s="5">
         <v>123</v>
       </c>
@@ -2986,13 +2997,13 @@
         <v>11</v>
       </c>
       <c r="F38" s="6">
-        <v>164</v>
+        <v>198</v>
       </c>
       <c r="G38" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" ht="18.35" customHeight="1">
       <c r="A39" t="s" s="5">
         <v>126</v>
       </c>
@@ -3000,7 +3011,7 @@
         <v>127</v>
       </c>
       <c r="C39" t="s" s="5">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="D39" t="s" s="5">
         <v>10</v>
@@ -3009,36 +3020,36 @@
         <v>11</v>
       </c>
       <c r="F39" s="6">
+        <v>164</v>
+      </c>
+      <c r="G39" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" ht="18.35" customHeight="1">
+      <c r="A40" t="s" s="5">
+        <v>129</v>
+      </c>
+      <c r="B40" t="s" s="5">
+        <v>130</v>
+      </c>
+      <c r="C40" t="s" s="5">
+        <v>117</v>
+      </c>
+      <c r="D40" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="E40" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F40" s="6">
         <v>170</v>
       </c>
-      <c r="G39" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" ht="50.35" customHeight="1">
-      <c r="A40" t="s" s="5">
-        <v>128</v>
-      </c>
-      <c r="B40" t="s" s="5">
-        <v>129</v>
-      </c>
-      <c r="C40" t="s" s="5">
-        <v>130</v>
-      </c>
-      <c r="D40" t="s" s="5">
-        <v>10</v>
-      </c>
-      <c r="E40" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F40" s="6">
-        <v>178</v>
-      </c>
       <c r="G40" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" ht="18.35" customHeight="1">
       <c r="A41" t="s" s="5">
         <v>131</v>
       </c>
@@ -3058,10 +3069,10 @@
         <v>178</v>
       </c>
       <c r="G41" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" ht="18.35" customHeight="1">
       <c r="A42" t="s" s="5">
         <v>134</v>
       </c>
@@ -3078,13 +3089,13 @@
         <v>11</v>
       </c>
       <c r="F42" s="6">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G42" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" ht="18.35" customHeight="1">
       <c r="A43" t="s" s="5">
         <v>137</v>
       </c>
@@ -3101,13 +3112,13 @@
         <v>11</v>
       </c>
       <c r="F43" s="6">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="G43" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" ht="18.35" customHeight="1">
       <c r="A44" t="s" s="5">
         <v>140</v>
       </c>
@@ -3124,13 +3135,13 @@
         <v>11</v>
       </c>
       <c r="F44" s="6">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="G44" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" ht="18.35" customHeight="1">
       <c r="A45" t="s" s="5">
         <v>143</v>
       </c>
@@ -3138,7 +3149,7 @@
         <v>144</v>
       </c>
       <c r="C45" t="s" s="5">
-        <v>79</v>
+        <v>145</v>
       </c>
       <c r="D45" t="s" s="5">
         <v>10</v>
@@ -3147,36 +3158,36 @@
         <v>11</v>
       </c>
       <c r="F45" s="6">
+        <v>176</v>
+      </c>
+      <c r="G45" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" ht="18.35" customHeight="1">
+      <c r="A46" t="s" s="5">
+        <v>146</v>
+      </c>
+      <c r="B46" t="s" s="5">
+        <v>147</v>
+      </c>
+      <c r="C46" t="s" s="5">
+        <v>82</v>
+      </c>
+      <c r="D46" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="E46" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F46" s="6">
         <v>170</v>
       </c>
-      <c r="G45" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" ht="50.35" customHeight="1">
-      <c r="A46" t="s" s="5">
-        <v>145</v>
-      </c>
-      <c r="B46" t="s" s="5">
-        <v>146</v>
-      </c>
-      <c r="C46" t="s" s="5">
-        <v>147</v>
-      </c>
-      <c r="D46" t="s" s="5">
-        <v>10</v>
-      </c>
-      <c r="E46" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F46" s="6">
-        <v>153</v>
-      </c>
       <c r="G46" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" ht="18.35" customHeight="1">
       <c r="A47" t="s" s="5">
         <v>148</v>
       </c>
@@ -3193,13 +3204,13 @@
         <v>11</v>
       </c>
       <c r="F47" s="6">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G47" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" ht="18.35" customHeight="1">
       <c r="A48" t="s" s="5">
         <v>151</v>
       </c>
@@ -3216,13 +3227,13 @@
         <v>11</v>
       </c>
       <c r="F48" s="6">
-        <v>213</v>
+        <v>158</v>
       </c>
       <c r="G48" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" ht="18.35" customHeight="1">
       <c r="A49" t="s" s="5">
         <v>154</v>
       </c>
@@ -3239,13 +3250,13 @@
         <v>11</v>
       </c>
       <c r="F49" s="6">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G49" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" ht="18.35" customHeight="1">
       <c r="A50" t="s" s="5">
         <v>157</v>
       </c>
@@ -3262,13 +3273,13 @@
         <v>11</v>
       </c>
       <c r="F50" s="6">
-        <v>170</v>
+        <v>215</v>
       </c>
       <c r="G50" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" ht="18.35" customHeight="1">
       <c r="A51" t="s" s="5">
         <v>160</v>
       </c>
@@ -3285,13 +3296,13 @@
         <v>11</v>
       </c>
       <c r="F51" s="6">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G51" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" ht="18.35" customHeight="1">
       <c r="A52" t="s" s="5">
         <v>163</v>
       </c>
@@ -3308,13 +3319,13 @@
         <v>11</v>
       </c>
       <c r="F52" s="6">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="G52" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" ht="18.35" customHeight="1">
       <c r="A53" t="s" s="5">
         <v>166</v>
       </c>
@@ -3331,13 +3342,13 @@
         <v>11</v>
       </c>
       <c r="F53" s="6">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="G53" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" ht="18.35" customHeight="1">
       <c r="A54" t="s" s="5">
         <v>169</v>
       </c>
@@ -3354,13 +3365,13 @@
         <v>11</v>
       </c>
       <c r="F54" s="6">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G54" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" ht="18.35" customHeight="1">
       <c r="A55" t="s" s="5">
         <v>172</v>
       </c>
@@ -3377,13 +3388,13 @@
         <v>11</v>
       </c>
       <c r="F55" s="6">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="G55" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" ht="18.35" customHeight="1">
       <c r="A56" t="s" s="5">
         <v>175</v>
       </c>
@@ -3400,13 +3411,13 @@
         <v>11</v>
       </c>
       <c r="F56" s="6">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="G56" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" ht="18.35" customHeight="1">
       <c r="A57" t="s" s="5">
         <v>178</v>
       </c>
@@ -3414,7 +3425,7 @@
         <v>179</v>
       </c>
       <c r="C57" t="s" s="5">
-        <v>139</v>
+        <v>180</v>
       </c>
       <c r="D57" t="s" s="5">
         <v>10</v>
@@ -3423,36 +3434,36 @@
         <v>11</v>
       </c>
       <c r="F57" s="6">
+        <v>190</v>
+      </c>
+      <c r="G57" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" ht="18.35" customHeight="1">
+      <c r="A58" t="s" s="5">
+        <v>181</v>
+      </c>
+      <c r="B58" t="s" s="5">
+        <v>182</v>
+      </c>
+      <c r="C58" t="s" s="5">
+        <v>142</v>
+      </c>
+      <c r="D58" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="E58" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F58" s="6">
         <v>188</v>
       </c>
-      <c r="G57" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="58" ht="50.35" customHeight="1">
-      <c r="A58" t="s" s="5">
-        <v>180</v>
-      </c>
-      <c r="B58" t="s" s="5">
-        <v>181</v>
-      </c>
-      <c r="C58" t="s" s="5">
-        <v>182</v>
-      </c>
-      <c r="D58" t="s" s="5">
-        <v>10</v>
-      </c>
-      <c r="E58" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F58" s="6">
-        <v>171</v>
-      </c>
       <c r="G58" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" ht="18.35" customHeight="1">
       <c r="A59" t="s" s="5">
         <v>183</v>
       </c>
@@ -3469,13 +3480,13 @@
         <v>11</v>
       </c>
       <c r="F59" s="6">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="G59" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="60" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" ht="18.35" customHeight="1">
       <c r="A60" t="s" s="5">
         <v>186</v>
       </c>
@@ -3492,13 +3503,13 @@
         <v>11</v>
       </c>
       <c r="F60" s="6">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G60" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" ht="18.35" customHeight="1">
       <c r="A61" t="s" s="5">
         <v>189</v>
       </c>
@@ -3515,13 +3526,13 @@
         <v>11</v>
       </c>
       <c r="F61" s="6">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="G61" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" ht="18.35" customHeight="1">
       <c r="A62" t="s" s="5">
         <v>192</v>
       </c>
@@ -3541,10 +3552,10 @@
         <v>175</v>
       </c>
       <c r="G62" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" ht="18.35" customHeight="1">
       <c r="A63" t="s" s="5">
         <v>195</v>
       </c>
@@ -3561,13 +3572,13 @@
         <v>11</v>
       </c>
       <c r="F63" s="6">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="G63" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="64" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" ht="18.35" customHeight="1">
       <c r="A64" t="s" s="5">
         <v>198</v>
       </c>
@@ -3584,13 +3595,13 @@
         <v>11</v>
       </c>
       <c r="F64" s="6">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="G64" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="65" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" ht="18.35" customHeight="1">
       <c r="A65" t="s" s="5">
         <v>201</v>
       </c>
@@ -3607,13 +3618,13 @@
         <v>11</v>
       </c>
       <c r="F65" s="6">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G65" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" ht="18.35" customHeight="1">
       <c r="A66" t="s" s="5">
         <v>204</v>
       </c>
@@ -3630,13 +3641,13 @@
         <v>11</v>
       </c>
       <c r="F66" s="6">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="G66" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="67" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" ht="18.35" customHeight="1">
       <c r="A67" t="s" s="5">
         <v>207</v>
       </c>
@@ -3647,180 +3658,180 @@
         <v>209</v>
       </c>
       <c r="D67" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="E67" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F67" s="6">
+        <v>182</v>
+      </c>
+      <c r="G67" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="68" ht="18.35" customHeight="1">
+      <c r="A68" t="s" s="5">
         <v>210</v>
       </c>
-      <c r="E67" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F67" s="6">
+      <c r="B68" t="s" s="5">
+        <v>211</v>
+      </c>
+      <c r="C68" t="s" s="5">
+        <v>212</v>
+      </c>
+      <c r="D68" t="s" s="5">
+        <v>213</v>
+      </c>
+      <c r="E68" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F68" s="6">
         <v>180</v>
       </c>
-      <c r="G67" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="68" ht="50.35" customHeight="1">
-      <c r="A68" t="s" s="5">
-        <v>211</v>
-      </c>
-      <c r="B68" t="s" s="5">
-        <v>212</v>
-      </c>
-      <c r="C68" t="s" s="5">
-        <v>213</v>
-      </c>
-      <c r="D68" t="s" s="5">
+      <c r="G68" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" ht="18.35" customHeight="1">
+      <c r="A69" t="s" s="5">
         <v>214</v>
       </c>
-      <c r="E68" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F68" s="6">
+      <c r="B69" t="s" s="5">
+        <v>215</v>
+      </c>
+      <c r="C69" t="s" s="5">
+        <v>216</v>
+      </c>
+      <c r="D69" t="s" s="5">
+        <v>217</v>
+      </c>
+      <c r="E69" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F69" s="6">
         <v>181</v>
       </c>
-      <c r="G68" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="69" ht="50.35" customHeight="1">
-      <c r="A69" t="s" s="5">
-        <v>215</v>
-      </c>
-      <c r="B69" t="s" s="5">
-        <v>216</v>
-      </c>
-      <c r="C69" t="s" s="5">
-        <v>76</v>
-      </c>
-      <c r="D69" t="s" s="5">
-        <v>214</v>
-      </c>
-      <c r="E69" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F69" s="6">
+      <c r="G69" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" ht="18.35" customHeight="1">
+      <c r="A70" t="s" s="5">
+        <v>218</v>
+      </c>
+      <c r="B70" t="s" s="5">
+        <v>219</v>
+      </c>
+      <c r="C70" t="s" s="5">
+        <v>79</v>
+      </c>
+      <c r="D70" t="s" s="5">
+        <v>217</v>
+      </c>
+      <c r="E70" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F70" s="6">
         <v>167</v>
       </c>
-      <c r="G69" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="70" ht="50.35" customHeight="1">
-      <c r="A70" t="s" s="5">
+      <c r="G70" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" ht="18.35" customHeight="1">
+      <c r="A71" t="s" s="5">
+        <v>220</v>
+      </c>
+      <c r="B71" t="s" s="5">
+        <v>221</v>
+      </c>
+      <c r="C71" t="s" s="5">
+        <v>222</v>
+      </c>
+      <c r="D71" t="s" s="5">
+        <v>223</v>
+      </c>
+      <c r="E71" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F71" s="6">
+        <v>240</v>
+      </c>
+      <c r="G71" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" ht="18.35" customHeight="1">
+      <c r="A72" t="s" s="5">
+        <v>224</v>
+      </c>
+      <c r="B72" t="s" s="5">
+        <v>225</v>
+      </c>
+      <c r="C72" t="s" s="5">
+        <v>191</v>
+      </c>
+      <c r="D72" t="s" s="5">
         <v>217</v>
       </c>
-      <c r="B70" t="s" s="5">
-        <v>218</v>
-      </c>
-      <c r="C70" t="s" s="5">
-        <v>219</v>
-      </c>
-      <c r="D70" t="s" s="5">
-        <v>220</v>
-      </c>
-      <c r="E70" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F70" s="6">
-        <v>240</v>
-      </c>
-      <c r="G70" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="71" ht="50.35" customHeight="1">
-      <c r="A71" t="s" s="5">
-        <v>221</v>
-      </c>
-      <c r="B71" t="s" s="5">
-        <v>222</v>
-      </c>
-      <c r="C71" t="s" s="5">
-        <v>188</v>
-      </c>
-      <c r="D71" t="s" s="5">
-        <v>214</v>
-      </c>
-      <c r="E71" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F71" s="6">
+      <c r="E72" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F72" s="6">
         <v>174</v>
       </c>
-      <c r="G71" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" ht="50.35" customHeight="1">
-      <c r="A72" t="s" s="5">
-        <v>223</v>
-      </c>
-      <c r="B72" t="s" s="5">
-        <v>224</v>
-      </c>
-      <c r="C72" t="s" s="5">
-        <v>225</v>
-      </c>
-      <c r="D72" t="s" s="5">
+      <c r="G72" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" ht="18.35" customHeight="1">
+      <c r="A73" t="s" s="5">
         <v>226</v>
       </c>
-      <c r="E72" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F72" s="6">
+      <c r="B73" t="s" s="5">
+        <v>227</v>
+      </c>
+      <c r="C73" t="s" s="5">
+        <v>228</v>
+      </c>
+      <c r="D73" t="s" s="5">
+        <v>229</v>
+      </c>
+      <c r="E73" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F73" s="6">
         <v>201</v>
       </c>
-      <c r="G72" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="73" ht="50.35" customHeight="1">
-      <c r="A73" t="s" s="5">
-        <v>227</v>
-      </c>
-      <c r="B73" t="s" s="5">
-        <v>228</v>
-      </c>
-      <c r="C73" t="s" s="5">
-        <v>229</v>
-      </c>
-      <c r="D73" t="s" s="5">
+      <c r="G73" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" ht="18.35" customHeight="1">
+      <c r="A74" t="s" s="5">
         <v>230</v>
       </c>
-      <c r="E73" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F73" s="6">
+      <c r="B74" t="s" s="5">
+        <v>231</v>
+      </c>
+      <c r="C74" t="s" s="5">
+        <v>232</v>
+      </c>
+      <c r="D74" t="s" s="5">
+        <v>233</v>
+      </c>
+      <c r="E74" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F74" s="6">
         <v>180</v>
       </c>
-      <c r="G73" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="74" ht="50.35" customHeight="1">
-      <c r="A74" t="s" s="5">
-        <v>231</v>
-      </c>
-      <c r="B74" t="s" s="5">
-        <v>232</v>
-      </c>
-      <c r="C74" t="s" s="5">
-        <v>233</v>
-      </c>
-      <c r="D74" t="s" s="5">
-        <v>230</v>
-      </c>
-      <c r="E74" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F74" s="6">
-        <v>170</v>
-      </c>
       <c r="G74" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="75" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" ht="18.35" customHeight="1">
       <c r="A75" t="s" s="5">
         <v>234</v>
       </c>
@@ -3831,19 +3842,19 @@
         <v>236</v>
       </c>
       <c r="D75" t="s" s="5">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E75" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F75" s="6">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="G75" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="76" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" ht="18.35" customHeight="1">
       <c r="A76" t="s" s="5">
         <v>237</v>
       </c>
@@ -3854,19 +3865,19 @@
         <v>239</v>
       </c>
       <c r="D76" t="s" s="5">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E76" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F76" s="6">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="G76" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="77" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" ht="18.35" customHeight="1">
       <c r="A77" t="s" s="5">
         <v>240</v>
       </c>
@@ -3877,19 +3888,19 @@
         <v>242</v>
       </c>
       <c r="D77" t="s" s="5">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E77" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F77" s="6">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="G77" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="78" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" ht="18.35" customHeight="1">
       <c r="A78" t="s" s="5">
         <v>243</v>
       </c>
@@ -3900,65 +3911,65 @@
         <v>245</v>
       </c>
       <c r="D78" t="s" s="5">
+        <v>233</v>
+      </c>
+      <c r="E78" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F78" s="6">
+        <v>190</v>
+      </c>
+      <c r="G78" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" ht="18.35" customHeight="1">
+      <c r="A79" t="s" s="5">
         <v>246</v>
       </c>
-      <c r="E78" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F78" s="6">
+      <c r="B79" t="s" s="5">
+        <v>247</v>
+      </c>
+      <c r="C79" t="s" s="5">
+        <v>248</v>
+      </c>
+      <c r="D79" t="s" s="5">
+        <v>249</v>
+      </c>
+      <c r="E79" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F79" s="6">
         <v>150</v>
       </c>
-      <c r="G78" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="79" ht="50.35" customHeight="1">
-      <c r="A79" t="s" s="5">
-        <v>247</v>
-      </c>
-      <c r="B79" t="s" s="5">
-        <v>248</v>
-      </c>
-      <c r="C79" t="s" s="5">
-        <v>50</v>
-      </c>
-      <c r="D79" t="s" s="5">
-        <v>230</v>
-      </c>
-      <c r="E79" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F79" s="6">
+      <c r="G79" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="80" ht="18.35" customHeight="1">
+      <c r="A80" t="s" s="5">
+        <v>250</v>
+      </c>
+      <c r="B80" t="s" s="5">
+        <v>251</v>
+      </c>
+      <c r="C80" t="s" s="5">
+        <v>53</v>
+      </c>
+      <c r="D80" t="s" s="5">
+        <v>233</v>
+      </c>
+      <c r="E80" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F80" s="6">
         <v>200</v>
       </c>
-      <c r="G79" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" ht="50.35" customHeight="1">
-      <c r="A80" t="s" s="5">
-        <v>249</v>
-      </c>
-      <c r="B80" t="s" s="5">
-        <v>250</v>
-      </c>
-      <c r="C80" t="s" s="5">
-        <v>251</v>
-      </c>
-      <c r="D80" t="s" s="5">
-        <v>246</v>
-      </c>
-      <c r="E80" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F80" s="6">
-        <v>150</v>
-      </c>
       <c r="G80" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="81" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" ht="18.35" customHeight="1">
       <c r="A81" t="s" s="5">
         <v>252</v>
       </c>
@@ -3969,7 +3980,7 @@
         <v>254</v>
       </c>
       <c r="D81" t="s" s="5">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="E81" t="s" s="5">
         <v>11</v>
@@ -3978,10 +3989,10 @@
         <v>150</v>
       </c>
       <c r="G81" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="82" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" ht="18.35" customHeight="1">
       <c r="A82" t="s" s="5">
         <v>255</v>
       </c>
@@ -3992,42 +4003,42 @@
         <v>257</v>
       </c>
       <c r="D82" t="s" s="5">
+        <v>249</v>
+      </c>
+      <c r="E82" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F82" s="6">
+        <v>150</v>
+      </c>
+      <c r="G82" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="83" ht="18.35" customHeight="1">
+      <c r="A83" t="s" s="5">
         <v>258</v>
       </c>
-      <c r="E82" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F82" s="6">
+      <c r="B83" t="s" s="5">
+        <v>259</v>
+      </c>
+      <c r="C83" t="s" s="5">
+        <v>260</v>
+      </c>
+      <c r="D83" t="s" s="5">
+        <v>261</v>
+      </c>
+      <c r="E83" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F83" s="6">
         <v>170</v>
       </c>
-      <c r="G82" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="83" ht="50.35" customHeight="1">
-      <c r="A83" t="s" s="5">
-        <v>259</v>
-      </c>
-      <c r="B83" t="s" s="5">
-        <v>260</v>
-      </c>
-      <c r="C83" t="s" s="5">
-        <v>261</v>
-      </c>
-      <c r="D83" t="s" s="5">
-        <v>226</v>
-      </c>
-      <c r="E83" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F83" s="6">
-        <v>209</v>
-      </c>
       <c r="G83" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="84" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="84" ht="18.35" customHeight="1">
       <c r="A84" t="s" s="5">
         <v>262</v>
       </c>
@@ -4038,19 +4049,19 @@
         <v>264</v>
       </c>
       <c r="D84" t="s" s="5">
-        <v>210</v>
+        <v>229</v>
       </c>
       <c r="E84" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F84" s="6">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="G84" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="85" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85" ht="18.35" customHeight="1">
       <c r="A85" t="s" s="5">
         <v>265</v>
       </c>
@@ -4061,19 +4072,19 @@
         <v>267</v>
       </c>
       <c r="D85" t="s" s="5">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E85" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F85" s="6">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="G85" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="86" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" ht="18.35" customHeight="1">
       <c r="A86" t="s" s="5">
         <v>268</v>
       </c>
@@ -4084,19 +4095,19 @@
         <v>270</v>
       </c>
       <c r="D86" t="s" s="5">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="E86" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F86" s="6">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G86" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="87" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="87" ht="18.35" customHeight="1">
       <c r="A87" t="s" s="5">
         <v>271</v>
       </c>
@@ -4107,19 +4118,19 @@
         <v>273</v>
       </c>
       <c r="D87" t="s" s="5">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E87" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F87" s="6">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="G87" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="88" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="88" ht="18.35" customHeight="1">
       <c r="A88" t="s" s="5">
         <v>274</v>
       </c>
@@ -4130,19 +4141,19 @@
         <v>276</v>
       </c>
       <c r="D88" t="s" s="5">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E88" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F88" s="6">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="G88" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="89" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="89" ht="18.35" customHeight="1">
       <c r="A89" t="s" s="5">
         <v>277</v>
       </c>
@@ -4153,19 +4164,19 @@
         <v>279</v>
       </c>
       <c r="D89" t="s" s="5">
-        <v>10</v>
+        <v>223</v>
       </c>
       <c r="E89" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F89" s="6">
-        <v>175</v>
+        <v>219</v>
       </c>
       <c r="G89" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="90" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" ht="18.35" customHeight="1">
       <c r="A90" t="s" s="5">
         <v>280</v>
       </c>
@@ -4182,13 +4193,13 @@
         <v>11</v>
       </c>
       <c r="F90" s="6">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="G90" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="91" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" ht="18.35" customHeight="1">
       <c r="A91" t="s" s="5">
         <v>283</v>
       </c>
@@ -4205,13 +4216,13 @@
         <v>11</v>
       </c>
       <c r="F91" s="6">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="G91" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="92" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92" ht="18.35" customHeight="1">
       <c r="A92" t="s" s="5">
         <v>286</v>
       </c>
@@ -4228,13 +4239,13 @@
         <v>11</v>
       </c>
       <c r="F92" s="6">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="G92" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="93" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="93" ht="18.35" customHeight="1">
       <c r="A93" t="s" s="5">
         <v>289</v>
       </c>
@@ -4251,13 +4262,13 @@
         <v>11</v>
       </c>
       <c r="F93" s="6">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="G93" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="94" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="94" ht="18.35" customHeight="1">
       <c r="A94" t="s" s="5">
         <v>292</v>
       </c>
@@ -4274,13 +4285,13 @@
         <v>11</v>
       </c>
       <c r="F94" s="6">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="G94" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="95" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="95" ht="18.35" customHeight="1">
       <c r="A95" t="s" s="5">
         <v>295</v>
       </c>
@@ -4291,19 +4302,19 @@
         <v>297</v>
       </c>
       <c r="D95" t="s" s="5">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="E95" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F95" s="6">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="G95" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="96" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="96" ht="18.35" customHeight="1">
       <c r="A96" t="s" s="5">
         <v>298</v>
       </c>
@@ -4314,7 +4325,7 @@
         <v>300</v>
       </c>
       <c r="D96" t="s" s="5">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E96" t="s" s="5">
         <v>11</v>
@@ -4323,10 +4334,10 @@
         <v>174</v>
       </c>
       <c r="G96" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="97" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="97" ht="18.35" customHeight="1">
       <c r="A97" t="s" s="5">
         <v>301</v>
       </c>
@@ -4334,10 +4345,10 @@
         <v>302</v>
       </c>
       <c r="C97" t="s" s="5">
-        <v>191</v>
+        <v>303</v>
       </c>
       <c r="D97" t="s" s="5">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E97" t="s" s="5">
         <v>11</v>
@@ -4346,56 +4357,56 @@
         <v>174</v>
       </c>
       <c r="G97" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="98" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="98" ht="18.35" customHeight="1">
       <c r="A98" t="s" s="5">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B98" t="s" s="5">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C98" t="s" s="5">
-        <v>102</v>
+        <v>194</v>
       </c>
       <c r="D98" t="s" s="5">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E98" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F98" s="6">
+        <v>174</v>
+      </c>
+      <c r="G98" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="99" ht="18.35" customHeight="1">
+      <c r="A99" t="s" s="5">
+        <v>306</v>
+      </c>
+      <c r="B99" t="s" s="5">
+        <v>307</v>
+      </c>
+      <c r="C99" t="s" s="5">
+        <v>105</v>
+      </c>
+      <c r="D99" t="s" s="5">
+        <v>44</v>
+      </c>
+      <c r="E99" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F99" s="6">
         <v>172</v>
       </c>
-      <c r="G98" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="99" ht="50.35" customHeight="1">
-      <c r="A99" t="s" s="5">
-        <v>305</v>
-      </c>
-      <c r="B99" t="s" s="5">
-        <v>306</v>
-      </c>
-      <c r="C99" t="s" s="5">
-        <v>307</v>
-      </c>
-      <c r="D99" t="s" s="5">
-        <v>41</v>
-      </c>
-      <c r="E99" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F99" s="6">
-        <v>180</v>
-      </c>
       <c r="G99" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="100" ht="50.35" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" ht="18.35" customHeight="1">
       <c r="A100" t="s" s="5">
         <v>308</v>
       </c>
@@ -4403,29 +4414,52 @@
         <v>309</v>
       </c>
       <c r="C100" t="s" s="5">
-        <v>219</v>
+        <v>310</v>
       </c>
       <c r="D100" t="s" s="5">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E100" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F100" s="6">
+        <v>180</v>
+      </c>
+      <c r="G100" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="101" ht="18.35" customHeight="1">
+      <c r="A101" t="s" s="5">
+        <v>311</v>
+      </c>
+      <c r="B101" t="s" s="5">
+        <v>312</v>
+      </c>
+      <c r="C101" t="s" s="5">
+        <v>222</v>
+      </c>
+      <c r="D101" t="s" s="5">
+        <v>44</v>
+      </c>
+      <c r="E101" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F101" s="6">
         <v>175</v>
       </c>
-      <c r="G100" t="s" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="101" ht="20.05" customHeight="1">
-      <c r="A101" s="7"/>
-      <c r="B101" s="7"/>
-      <c r="C101" s="7"/>
-      <c r="D101" s="7"/>
-      <c r="E101" s="7"/>
-      <c r="F101" s="7"/>
-      <c r="G101" s="7"/>
+      <c r="G101" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="102" ht="20.05" customHeight="1">
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="7"/>
+      <c r="E102" s="7"/>
+      <c r="F102" s="7"/>
+      <c r="G102" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>

<commit_message>
Add trophies and personal awards into each player of the team.
</commit_message>
<xml_diff>
--- a/player_info.xlsx
+++ b/player_info.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="384">
   <si>
     <t>name</t>
   </si>
@@ -79,6 +79,15 @@
     <t>1900-1-9</t>
   </si>
   <si>
+    <t>Rokusuke Koenji</t>
+  </si>
+  <si>
+    <t>cote_3</t>
+  </si>
+  <si>
+    <t>1900-3-4</t>
+  </si>
+  <si>
     <t>Eren Yeager</t>
   </si>
   <si>
@@ -950,6 +959,210 @@
   </si>
   <si>
     <t>u_and_i_1</t>
+  </si>
+  <si>
+    <t>Saitama</t>
+  </si>
+  <si>
+    <t>opm_9</t>
+  </si>
+  <si>
+    <t>1900-4-21</t>
+  </si>
+  <si>
+    <t>Genos</t>
+  </si>
+  <si>
+    <t>opm_10</t>
+  </si>
+  <si>
+    <t>1900-10-10</t>
+  </si>
+  <si>
+    <t>Sonic</t>
+  </si>
+  <si>
+    <t>opm_7</t>
+  </si>
+  <si>
+    <t>1900-10-5</t>
+  </si>
+  <si>
+    <t>Garou</t>
+  </si>
+  <si>
+    <t>opm_11</t>
+  </si>
+  <si>
+    <t>1900-9-4</t>
+  </si>
+  <si>
+    <t>Flashy Flash</t>
+  </si>
+  <si>
+    <t>opm_13</t>
+  </si>
+  <si>
+    <t>1900-3-11</t>
+  </si>
+  <si>
+    <t>King</t>
+  </si>
+  <si>
+    <t>opm_1</t>
+  </si>
+  <si>
+    <t>1900-11-10</t>
+  </si>
+  <si>
+    <t>Shinnosuke Nohara</t>
+  </si>
+  <si>
+    <t>csc_10</t>
+  </si>
+  <si>
+    <t>Kagura Karatachi</t>
+  </si>
+  <si>
+    <t>csc_8</t>
+  </si>
+  <si>
+    <t>1900-9-20</t>
+  </si>
+  <si>
+    <t>Kirigakure</t>
+  </si>
+  <si>
+    <t>Kirigaya Kazuto</t>
+  </si>
+  <si>
+    <t>csc_7</t>
+  </si>
+  <si>
+    <t>1900-10-7</t>
+  </si>
+  <si>
+    <t>Murkrow</t>
+  </si>
+  <si>
+    <t>csc_11</t>
+  </si>
+  <si>
+    <t>Johto</t>
+  </si>
+  <si>
+    <t>Sudowoodo</t>
+  </si>
+  <si>
+    <t>csc_1</t>
+  </si>
+  <si>
+    <t>1900-8-31</t>
+  </si>
+  <si>
+    <t>Itadori Yuuji</t>
+  </si>
+  <si>
+    <t>jjk_10</t>
+  </si>
+  <si>
+    <t>Megumi Fushiguro</t>
+  </si>
+  <si>
+    <t>jjk_7</t>
+  </si>
+  <si>
+    <t>1900-12-22</t>
+  </si>
+  <si>
+    <t>Inumaki Toge</t>
+  </si>
+  <si>
+    <t>jjk_8</t>
+  </si>
+  <si>
+    <t>1900-10-23</t>
+  </si>
+  <si>
+    <t>Yuta Okkotsu</t>
+  </si>
+  <si>
+    <t>jjk_11</t>
+  </si>
+  <si>
+    <t>1900-3-7</t>
+  </si>
+  <si>
+    <t>Gojo Satoru</t>
+  </si>
+  <si>
+    <t>jjk_25</t>
+  </si>
+  <si>
+    <t>L Lawliet</t>
+  </si>
+  <si>
+    <t>dn_10</t>
+  </si>
+  <si>
+    <t>Light Yagami</t>
+  </si>
+  <si>
+    <t>dn_7</t>
+  </si>
+  <si>
+    <t>1900-2-28</t>
+  </si>
+  <si>
+    <t>Ryuk</t>
+  </si>
+  <si>
+    <t>dn_1</t>
+  </si>
+  <si>
+    <t>1900-12-3</t>
+  </si>
+  <si>
+    <t>Nate River</t>
+  </si>
+  <si>
+    <t>dn_6</t>
+  </si>
+  <si>
+    <t>1900-8-24</t>
+  </si>
+  <si>
+    <t>Ken Sudo</t>
+  </si>
+  <si>
+    <t>efc_1</t>
+  </si>
+  <si>
+    <t>Haruki Yamauchi</t>
+  </si>
+  <si>
+    <t>efc_8</t>
+  </si>
+  <si>
+    <t>Ryomen Sukuna</t>
+  </si>
+  <si>
+    <t>efc_10</t>
+  </si>
+  <si>
+    <t>1900-11-1</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>efc_9</t>
+  </si>
+  <si>
+    <t>1900-2-12</t>
+  </si>
+  <si>
+    <t>Amegakure</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1256,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1064,6 +1277,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -2115,7 +2334,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:G164"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A2" xSplit="0" ySplit="1" activePane="bottomLeft" state="frozen"/>
@@ -2244,7 +2463,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" ht="18.35" customHeight="1">
+    <row r="6" ht="24.35" customHeight="1">
       <c r="A6" t="s" s="5">
         <v>22</v>
       </c>
@@ -2255,59 +2474,59 @@
         <v>24</v>
       </c>
       <c r="D6" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F6" s="6">
+        <v>181</v>
+      </c>
+      <c r="G6" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" ht="18.35" customHeight="1">
+      <c r="A7" t="s" s="5">
         <v>25</v>
       </c>
-      <c r="E6" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="B7" t="s" s="5">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s" s="5">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s" s="5">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F7" s="6">
         <v>183</v>
       </c>
-      <c r="G6" t="s" s="5">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" ht="34.35" customHeight="1">
-      <c r="A7" t="s" s="5">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s" s="5">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s" s="5">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s" s="5">
+      <c r="G7" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" ht="34.35" customHeight="1">
+      <c r="A8" t="s" s="5">
         <v>29</v>
       </c>
-      <c r="E7" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="B8" t="s" s="5">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s" s="5">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s" s="5">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F8" s="6">
         <v>160</v>
-      </c>
-      <c r="G7" t="s" s="5">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" ht="18.35" customHeight="1">
-      <c r="A8" t="s" s="5">
-        <v>30</v>
-      </c>
-      <c r="B8" t="s" s="5">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s" s="5">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s" s="5">
-        <v>25</v>
-      </c>
-      <c r="E8" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F8" s="6">
-        <v>169</v>
       </c>
       <c r="G8" t="s" s="5">
         <v>16</v>
@@ -2324,13 +2543,13 @@
         <v>35</v>
       </c>
       <c r="D9" t="s" s="5">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F9" s="6">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="G9" t="s" s="5">
         <v>16</v>
@@ -2338,22 +2557,22 @@
     </row>
     <row r="10" ht="18.35" customHeight="1">
       <c r="A10" t="s" s="5">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s" s="5">
         <v>37</v>
       </c>
-      <c r="B10" t="s" s="5">
+      <c r="C10" t="s" s="5">
         <v>38</v>
       </c>
-      <c r="C10" t="s" s="5">
+      <c r="D10" t="s" s="5">
         <v>39</v>
       </c>
-      <c r="D10" t="s" s="5">
-        <v>40</v>
-      </c>
       <c r="E10" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F10" s="6">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="G10" t="s" s="5">
         <v>16</v>
@@ -2361,22 +2580,22 @@
     </row>
     <row r="11" ht="18.35" customHeight="1">
       <c r="A11" t="s" s="5">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s" s="5">
         <v>41</v>
       </c>
-      <c r="B11" t="s" s="5">
+      <c r="C11" t="s" s="5">
         <v>42</v>
       </c>
-      <c r="C11" t="s" s="5">
+      <c r="D11" t="s" s="5">
         <v>43</v>
       </c>
-      <c r="D11" t="s" s="5">
-        <v>44</v>
-      </c>
       <c r="E11" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F11" s="6">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="G11" t="s" s="5">
         <v>16</v>
@@ -2384,22 +2603,22 @@
     </row>
     <row r="12" ht="18.35" customHeight="1">
       <c r="A12" t="s" s="5">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s" s="5">
         <v>45</v>
       </c>
-      <c r="B12" t="s" s="5">
+      <c r="C12" t="s" s="5">
         <v>46</v>
       </c>
-      <c r="C12" t="s" s="5">
+      <c r="D12" t="s" s="5">
         <v>47</v>
       </c>
-      <c r="D12" t="s" s="5">
-        <v>44</v>
-      </c>
       <c r="E12" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F12" s="6">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="G12" t="s" s="5">
         <v>16</v>
@@ -2416,13 +2635,13 @@
         <v>50</v>
       </c>
       <c r="D13" t="s" s="5">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F13" s="6">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="G13" t="s" s="5">
         <v>16</v>
@@ -2439,13 +2658,13 @@
         <v>53</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F14" s="6">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="G14" t="s" s="5">
         <v>16</v>
@@ -2462,13 +2681,13 @@
         <v>56</v>
       </c>
       <c r="D15" t="s" s="5">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F15" s="6">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="G15" t="s" s="5">
         <v>16</v>
@@ -2485,13 +2704,13 @@
         <v>59</v>
       </c>
       <c r="D16" t="s" s="5">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E16" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F16" s="6">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="G16" t="s" s="5">
         <v>16</v>
@@ -2499,22 +2718,22 @@
     </row>
     <row r="17" ht="18.35" customHeight="1">
       <c r="A17" t="s" s="5">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s" s="5">
         <v>61</v>
       </c>
-      <c r="B17" t="s" s="5">
+      <c r="C17" t="s" s="5">
         <v>62</v>
       </c>
-      <c r="C17" t="s" s="5">
+      <c r="D17" t="s" s="5">
         <v>63</v>
       </c>
-      <c r="D17" t="s" s="5">
-        <v>64</v>
-      </c>
       <c r="E17" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F17" s="6">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="G17" t="s" s="5">
         <v>16</v>
@@ -2522,16 +2741,16 @@
     </row>
     <row r="18" ht="18.35" customHeight="1">
       <c r="A18" t="s" s="5">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s" s="5">
         <v>65</v>
       </c>
-      <c r="B18" t="s" s="5">
+      <c r="C18" t="s" s="5">
         <v>66</v>
       </c>
-      <c r="C18" t="s" s="5">
+      <c r="D18" t="s" s="5">
         <v>67</v>
-      </c>
-      <c r="D18" t="s" s="5">
-        <v>60</v>
       </c>
       <c r="E18" t="s" s="5">
         <v>11</v>
@@ -2554,13 +2773,13 @@
         <v>70</v>
       </c>
       <c r="D19" t="s" s="5">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F19" s="6">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="G19" t="s" s="5">
         <v>16</v>
@@ -2577,13 +2796,13 @@
         <v>73</v>
       </c>
       <c r="D20" t="s" s="5">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F20" s="6">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G20" t="s" s="5">
         <v>16</v>
@@ -2600,13 +2819,13 @@
         <v>76</v>
       </c>
       <c r="D21" t="s" s="5">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E21" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F21" s="6">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="G21" t="s" s="5">
         <v>16</v>
@@ -2623,13 +2842,13 @@
         <v>79</v>
       </c>
       <c r="D22" t="s" s="5">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E22" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F22" s="6">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G22" t="s" s="5">
         <v>16</v>
@@ -2646,13 +2865,13 @@
         <v>82</v>
       </c>
       <c r="D23" t="s" s="5">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="E23" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F23" s="6">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G23" t="s" s="5">
         <v>16</v>
@@ -2675,7 +2894,7 @@
         <v>11</v>
       </c>
       <c r="F24" s="6">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G24" t="s" s="5">
         <v>16</v>
@@ -2698,7 +2917,7 @@
         <v>11</v>
       </c>
       <c r="F25" s="6">
-        <v>134</v>
+        <v>180</v>
       </c>
       <c r="G25" t="s" s="5">
         <v>16</v>
@@ -2721,13 +2940,13 @@
         <v>11</v>
       </c>
       <c r="F26" s="6">
-        <v>186</v>
+        <v>134</v>
       </c>
       <c r="G26" t="s" s="5">
         <v>16</v>
       </c>
     </row>
-    <row r="27" ht="34.35" customHeight="1">
+    <row r="27" ht="18.35" customHeight="1">
       <c r="A27" t="s" s="5">
         <v>92</v>
       </c>
@@ -2750,7 +2969,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" ht="18.35" customHeight="1">
+    <row r="28" ht="34.35" customHeight="1">
       <c r="A28" t="s" s="5">
         <v>95</v>
       </c>
@@ -2758,7 +2977,7 @@
         <v>96</v>
       </c>
       <c r="C28" t="s" s="5">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="D28" t="s" s="5">
         <v>10</v>
@@ -2767,7 +2986,7 @@
         <v>11</v>
       </c>
       <c r="F28" s="6">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="G28" t="s" s="5">
         <v>16</v>
@@ -2775,13 +2994,13 @@
     </row>
     <row r="29" ht="18.35" customHeight="1">
       <c r="A29" t="s" s="5">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B29" t="s" s="5">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s" s="5">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="D29" t="s" s="5">
         <v>10</v>
@@ -2790,7 +3009,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="6">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G29" t="s" s="5">
         <v>16</v>
@@ -2836,7 +3055,7 @@
         <v>11</v>
       </c>
       <c r="F31" s="6">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G31" t="s" s="5">
         <v>16</v>
@@ -2859,7 +3078,7 @@
         <v>11</v>
       </c>
       <c r="F32" s="6">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G32" t="s" s="5">
         <v>16</v>
@@ -2882,7 +3101,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="6">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="G33" t="s" s="5">
         <v>16</v>
@@ -2905,7 +3124,7 @@
         <v>11</v>
       </c>
       <c r="F34" s="6">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="G34" t="s" s="5">
         <v>16</v>
@@ -2928,7 +3147,7 @@
         <v>11</v>
       </c>
       <c r="F35" s="6">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="G35" t="s" s="5">
         <v>16</v>
@@ -2951,7 +3170,7 @@
         <v>11</v>
       </c>
       <c r="F36" s="6">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="G36" t="s" s="5">
         <v>16</v>
@@ -2965,7 +3184,7 @@
         <v>122</v>
       </c>
       <c r="C37" t="s" s="5">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="D37" t="s" s="5">
         <v>10</v>
@@ -2974,7 +3193,7 @@
         <v>11</v>
       </c>
       <c r="F37" s="6">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="G37" t="s" s="5">
         <v>16</v>
@@ -2982,13 +3201,13 @@
     </row>
     <row r="38" ht="18.35" customHeight="1">
       <c r="A38" t="s" s="5">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B38" t="s" s="5">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C38" t="s" s="5">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="D38" t="s" s="5">
         <v>10</v>
@@ -2997,7 +3216,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="6">
-        <v>198</v>
+        <v>165</v>
       </c>
       <c r="G38" t="s" s="5">
         <v>16</v>
@@ -3020,7 +3239,7 @@
         <v>11</v>
       </c>
       <c r="F39" s="6">
-        <v>164</v>
+        <v>198</v>
       </c>
       <c r="G39" t="s" s="5">
         <v>16</v>
@@ -3034,7 +3253,7 @@
         <v>130</v>
       </c>
       <c r="C40" t="s" s="5">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="D40" t="s" s="5">
         <v>10</v>
@@ -3043,7 +3262,7 @@
         <v>11</v>
       </c>
       <c r="F40" s="6">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G40" t="s" s="5">
         <v>16</v>
@@ -3051,13 +3270,13 @@
     </row>
     <row r="41" ht="18.35" customHeight="1">
       <c r="A41" t="s" s="5">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B41" t="s" s="5">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C41" t="s" s="5">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="D41" t="s" s="5">
         <v>10</v>
@@ -3066,7 +3285,7 @@
         <v>11</v>
       </c>
       <c r="F41" s="6">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="G41" t="s" s="5">
         <v>16</v>
@@ -3112,7 +3331,7 @@
         <v>11</v>
       </c>
       <c r="F43" s="6">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G43" t="s" s="5">
         <v>16</v>
@@ -3135,7 +3354,7 @@
         <v>11</v>
       </c>
       <c r="F44" s="6">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="G44" t="s" s="5">
         <v>16</v>
@@ -3158,7 +3377,7 @@
         <v>11</v>
       </c>
       <c r="F45" s="6">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="G45" t="s" s="5">
         <v>16</v>
@@ -3172,7 +3391,7 @@
         <v>147</v>
       </c>
       <c r="C46" t="s" s="5">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="D46" t="s" s="5">
         <v>10</v>
@@ -3181,7 +3400,7 @@
         <v>11</v>
       </c>
       <c r="F46" s="6">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="G46" t="s" s="5">
         <v>16</v>
@@ -3189,13 +3408,13 @@
     </row>
     <row r="47" ht="18.35" customHeight="1">
       <c r="A47" t="s" s="5">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B47" t="s" s="5">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C47" t="s" s="5">
-        <v>150</v>
+        <v>85</v>
       </c>
       <c r="D47" t="s" s="5">
         <v>10</v>
@@ -3204,7 +3423,7 @@
         <v>11</v>
       </c>
       <c r="F47" s="6">
-        <v>153</v>
+        <v>170</v>
       </c>
       <c r="G47" t="s" s="5">
         <v>16</v>
@@ -3227,7 +3446,7 @@
         <v>11</v>
       </c>
       <c r="F48" s="6">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G48" t="s" s="5">
         <v>16</v>
@@ -3250,7 +3469,7 @@
         <v>11</v>
       </c>
       <c r="F49" s="6">
-        <v>213</v>
+        <v>158</v>
       </c>
       <c r="G49" t="s" s="5">
         <v>16</v>
@@ -3273,7 +3492,7 @@
         <v>11</v>
       </c>
       <c r="F50" s="6">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G50" t="s" s="5">
         <v>16</v>
@@ -3296,7 +3515,7 @@
         <v>11</v>
       </c>
       <c r="F51" s="6">
-        <v>170</v>
+        <v>215</v>
       </c>
       <c r="G51" t="s" s="5">
         <v>16</v>
@@ -3319,7 +3538,7 @@
         <v>11</v>
       </c>
       <c r="F52" s="6">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G52" t="s" s="5">
         <v>16</v>
@@ -3342,7 +3561,7 @@
         <v>11</v>
       </c>
       <c r="F53" s="6">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="G53" t="s" s="5">
         <v>16</v>
@@ -3365,7 +3584,7 @@
         <v>11</v>
       </c>
       <c r="F54" s="6">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="G54" t="s" s="5">
         <v>16</v>
@@ -3388,7 +3607,7 @@
         <v>11</v>
       </c>
       <c r="F55" s="6">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G55" t="s" s="5">
         <v>16</v>
@@ -3411,7 +3630,7 @@
         <v>11</v>
       </c>
       <c r="F56" s="6">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="G56" t="s" s="5">
         <v>16</v>
@@ -3434,7 +3653,7 @@
         <v>11</v>
       </c>
       <c r="F57" s="6">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="G57" t="s" s="5">
         <v>16</v>
@@ -3448,7 +3667,7 @@
         <v>182</v>
       </c>
       <c r="C58" t="s" s="5">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="D58" t="s" s="5">
         <v>10</v>
@@ -3457,7 +3676,7 @@
         <v>11</v>
       </c>
       <c r="F58" s="6">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G58" t="s" s="5">
         <v>16</v>
@@ -3465,13 +3684,13 @@
     </row>
     <row r="59" ht="18.35" customHeight="1">
       <c r="A59" t="s" s="5">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B59" t="s" s="5">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C59" t="s" s="5">
-        <v>185</v>
+        <v>145</v>
       </c>
       <c r="D59" t="s" s="5">
         <v>10</v>
@@ -3480,7 +3699,7 @@
         <v>11</v>
       </c>
       <c r="F59" s="6">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="G59" t="s" s="5">
         <v>16</v>
@@ -3503,7 +3722,7 @@
         <v>11</v>
       </c>
       <c r="F60" s="6">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="G60" t="s" s="5">
         <v>16</v>
@@ -3526,7 +3745,7 @@
         <v>11</v>
       </c>
       <c r="F61" s="6">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G61" t="s" s="5">
         <v>16</v>
@@ -3549,7 +3768,7 @@
         <v>11</v>
       </c>
       <c r="F62" s="6">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="G62" t="s" s="5">
         <v>16</v>
@@ -3595,7 +3814,7 @@
         <v>11</v>
       </c>
       <c r="F64" s="6">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="G64" t="s" s="5">
         <v>16</v>
@@ -3618,7 +3837,7 @@
         <v>11</v>
       </c>
       <c r="F65" s="6">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="G65" t="s" s="5">
         <v>16</v>
@@ -3641,7 +3860,7 @@
         <v>11</v>
       </c>
       <c r="F66" s="6">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G66" t="s" s="5">
         <v>16</v>
@@ -3664,7 +3883,7 @@
         <v>11</v>
       </c>
       <c r="F67" s="6">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="G67" t="s" s="5">
         <v>16</v>
@@ -3681,13 +3900,13 @@
         <v>212</v>
       </c>
       <c r="D68" t="s" s="5">
-        <v>213</v>
+        <v>10</v>
       </c>
       <c r="E68" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F68" s="6">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="G68" t="s" s="5">
         <v>16</v>
@@ -3695,22 +3914,22 @@
     </row>
     <row r="69" ht="18.35" customHeight="1">
       <c r="A69" t="s" s="5">
+        <v>213</v>
+      </c>
+      <c r="B69" t="s" s="5">
         <v>214</v>
       </c>
-      <c r="B69" t="s" s="5">
+      <c r="C69" t="s" s="5">
         <v>215</v>
       </c>
-      <c r="C69" t="s" s="5">
+      <c r="D69" t="s" s="5">
         <v>216</v>
       </c>
-      <c r="D69" t="s" s="5">
-        <v>217</v>
-      </c>
       <c r="E69" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F69" s="6">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G69" t="s" s="5">
         <v>16</v>
@@ -3718,22 +3937,22 @@
     </row>
     <row r="70" ht="18.35" customHeight="1">
       <c r="A70" t="s" s="5">
+        <v>217</v>
+      </c>
+      <c r="B70" t="s" s="5">
         <v>218</v>
       </c>
-      <c r="B70" t="s" s="5">
+      <c r="C70" t="s" s="5">
         <v>219</v>
       </c>
-      <c r="C70" t="s" s="5">
-        <v>79</v>
-      </c>
       <c r="D70" t="s" s="5">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E70" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F70" s="6">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="G70" t="s" s="5">
         <v>16</v>
@@ -3741,22 +3960,22 @@
     </row>
     <row r="71" ht="18.35" customHeight="1">
       <c r="A71" t="s" s="5">
+        <v>221</v>
+      </c>
+      <c r="B71" t="s" s="5">
+        <v>222</v>
+      </c>
+      <c r="C71" t="s" s="5">
+        <v>82</v>
+      </c>
+      <c r="D71" t="s" s="5">
         <v>220</v>
       </c>
-      <c r="B71" t="s" s="5">
-        <v>221</v>
-      </c>
-      <c r="C71" t="s" s="5">
-        <v>222</v>
-      </c>
-      <c r="D71" t="s" s="5">
-        <v>223</v>
-      </c>
       <c r="E71" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F71" s="6">
-        <v>240</v>
+        <v>167</v>
       </c>
       <c r="G71" t="s" s="5">
         <v>16</v>
@@ -3764,22 +3983,22 @@
     </row>
     <row r="72" ht="18.35" customHeight="1">
       <c r="A72" t="s" s="5">
+        <v>223</v>
+      </c>
+      <c r="B72" t="s" s="5">
         <v>224</v>
       </c>
-      <c r="B72" t="s" s="5">
+      <c r="C72" t="s" s="5">
         <v>225</v>
       </c>
-      <c r="C72" t="s" s="5">
-        <v>191</v>
-      </c>
       <c r="D72" t="s" s="5">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="E72" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F72" s="6">
-        <v>174</v>
+        <v>240</v>
       </c>
       <c r="G72" t="s" s="5">
         <v>16</v>
@@ -3787,22 +4006,22 @@
     </row>
     <row r="73" ht="18.35" customHeight="1">
       <c r="A73" t="s" s="5">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B73" t="s" s="5">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C73" t="s" s="5">
-        <v>228</v>
+        <v>194</v>
       </c>
       <c r="D73" t="s" s="5">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="E73" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F73" s="6">
-        <v>201</v>
+        <v>174</v>
       </c>
       <c r="G73" t="s" s="5">
         <v>16</v>
@@ -3810,22 +4029,22 @@
     </row>
     <row r="74" ht="18.35" customHeight="1">
       <c r="A74" t="s" s="5">
+        <v>229</v>
+      </c>
+      <c r="B74" t="s" s="5">
         <v>230</v>
       </c>
-      <c r="B74" t="s" s="5">
+      <c r="C74" t="s" s="5">
         <v>231</v>
       </c>
-      <c r="C74" t="s" s="5">
+      <c r="D74" t="s" s="5">
         <v>232</v>
       </c>
-      <c r="D74" t="s" s="5">
-        <v>233</v>
-      </c>
       <c r="E74" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F74" s="6">
-        <v>180</v>
+        <v>201</v>
       </c>
       <c r="G74" t="s" s="5">
         <v>16</v>
@@ -3833,22 +4052,22 @@
     </row>
     <row r="75" ht="18.35" customHeight="1">
       <c r="A75" t="s" s="5">
+        <v>233</v>
+      </c>
+      <c r="B75" t="s" s="5">
         <v>234</v>
       </c>
-      <c r="B75" t="s" s="5">
+      <c r="C75" t="s" s="5">
         <v>235</v>
       </c>
-      <c r="C75" t="s" s="5">
+      <c r="D75" t="s" s="5">
         <v>236</v>
       </c>
-      <c r="D75" t="s" s="5">
-        <v>233</v>
-      </c>
       <c r="E75" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F75" s="6">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="G75" t="s" s="5">
         <v>16</v>
@@ -3865,13 +4084,13 @@
         <v>239</v>
       </c>
       <c r="D76" t="s" s="5">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="E76" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F76" s="6">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="G76" t="s" s="5">
         <v>16</v>
@@ -3888,13 +4107,13 @@
         <v>242</v>
       </c>
       <c r="D77" t="s" s="5">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="E77" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F77" s="6">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="G77" t="s" s="5">
         <v>16</v>
@@ -3911,13 +4130,13 @@
         <v>245</v>
       </c>
       <c r="D78" t="s" s="5">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="E78" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F78" s="6">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="G78" t="s" s="5">
         <v>16</v>
@@ -3934,13 +4153,13 @@
         <v>248</v>
       </c>
       <c r="D79" t="s" s="5">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="E79" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F79" s="6">
-        <v>150</v>
+        <v>190</v>
       </c>
       <c r="G79" t="s" s="5">
         <v>16</v>
@@ -3948,22 +4167,22 @@
     </row>
     <row r="80" ht="18.35" customHeight="1">
       <c r="A80" t="s" s="5">
+        <v>249</v>
+      </c>
+      <c r="B80" t="s" s="5">
         <v>250</v>
       </c>
-      <c r="B80" t="s" s="5">
+      <c r="C80" t="s" s="5">
         <v>251</v>
       </c>
-      <c r="C80" t="s" s="5">
-        <v>53</v>
-      </c>
       <c r="D80" t="s" s="5">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="E80" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F80" s="6">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="G80" t="s" s="5">
         <v>16</v>
@@ -3971,22 +4190,22 @@
     </row>
     <row r="81" ht="18.35" customHeight="1">
       <c r="A81" t="s" s="5">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B81" t="s" s="5">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C81" t="s" s="5">
-        <v>254</v>
+        <v>56</v>
       </c>
       <c r="D81" t="s" s="5">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="E81" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F81" s="6">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="G81" t="s" s="5">
         <v>16</v>
@@ -4003,7 +4222,7 @@
         <v>257</v>
       </c>
       <c r="D82" t="s" s="5">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E82" t="s" s="5">
         <v>11</v>
@@ -4026,13 +4245,13 @@
         <v>260</v>
       </c>
       <c r="D83" t="s" s="5">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="E83" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F83" s="6">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="G83" t="s" s="5">
         <v>16</v>
@@ -4040,22 +4259,22 @@
     </row>
     <row r="84" ht="18.35" customHeight="1">
       <c r="A84" t="s" s="5">
+        <v>261</v>
+      </c>
+      <c r="B84" t="s" s="5">
         <v>262</v>
       </c>
-      <c r="B84" t="s" s="5">
+      <c r="C84" t="s" s="5">
         <v>263</v>
       </c>
-      <c r="C84" t="s" s="5">
+      <c r="D84" t="s" s="5">
         <v>264</v>
       </c>
-      <c r="D84" t="s" s="5">
-        <v>229</v>
-      </c>
       <c r="E84" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F84" s="6">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="G84" t="s" s="5">
         <v>16</v>
@@ -4072,13 +4291,13 @@
         <v>267</v>
       </c>
       <c r="D85" t="s" s="5">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="E85" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F85" s="6">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="G85" t="s" s="5">
         <v>16</v>
@@ -4095,13 +4314,13 @@
         <v>270</v>
       </c>
       <c r="D86" t="s" s="5">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="E86" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F86" s="6">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="G86" t="s" s="5">
         <v>16</v>
@@ -4118,13 +4337,13 @@
         <v>273</v>
       </c>
       <c r="D87" t="s" s="5">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="E87" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F87" s="6">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G87" t="s" s="5">
         <v>16</v>
@@ -4141,13 +4360,13 @@
         <v>276</v>
       </c>
       <c r="D88" t="s" s="5">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E88" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F88" s="6">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="G88" t="s" s="5">
         <v>16</v>
@@ -4164,13 +4383,13 @@
         <v>279</v>
       </c>
       <c r="D89" t="s" s="5">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E89" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F89" s="6">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="G89" t="s" s="5">
         <v>16</v>
@@ -4187,13 +4406,13 @@
         <v>282</v>
       </c>
       <c r="D90" t="s" s="5">
-        <v>10</v>
+        <v>226</v>
       </c>
       <c r="E90" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F90" s="6">
-        <v>175</v>
+        <v>219</v>
       </c>
       <c r="G90" t="s" s="5">
         <v>16</v>
@@ -4216,7 +4435,7 @@
         <v>11</v>
       </c>
       <c r="F91" s="6">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="G91" t="s" s="5">
         <v>16</v>
@@ -4239,7 +4458,7 @@
         <v>11</v>
       </c>
       <c r="F92" s="6">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="G92" t="s" s="5">
         <v>16</v>
@@ -4262,7 +4481,7 @@
         <v>11</v>
       </c>
       <c r="F93" s="6">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="G93" t="s" s="5">
         <v>16</v>
@@ -4285,7 +4504,7 @@
         <v>11</v>
       </c>
       <c r="F94" s="6">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="G94" t="s" s="5">
         <v>16</v>
@@ -4308,7 +4527,7 @@
         <v>11</v>
       </c>
       <c r="F95" s="6">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="G95" t="s" s="5">
         <v>16</v>
@@ -4325,13 +4544,13 @@
         <v>300</v>
       </c>
       <c r="D96" t="s" s="5">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="E96" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F96" s="6">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="G96" t="s" s="5">
         <v>16</v>
@@ -4348,7 +4567,7 @@
         <v>303</v>
       </c>
       <c r="D97" t="s" s="5">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E97" t="s" s="5">
         <v>11</v>
@@ -4368,10 +4587,10 @@
         <v>305</v>
       </c>
       <c r="C98" t="s" s="5">
-        <v>194</v>
+        <v>306</v>
       </c>
       <c r="D98" t="s" s="5">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E98" t="s" s="5">
         <v>11</v>
@@ -4385,22 +4604,22 @@
     </row>
     <row r="99" ht="18.35" customHeight="1">
       <c r="A99" t="s" s="5">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B99" t="s" s="5">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C99" t="s" s="5">
-        <v>105</v>
+        <v>197</v>
       </c>
       <c r="D99" t="s" s="5">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E99" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F99" s="6">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G99" t="s" s="5">
         <v>16</v>
@@ -4408,22 +4627,22 @@
     </row>
     <row r="100" ht="18.35" customHeight="1">
       <c r="A100" t="s" s="5">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B100" t="s" s="5">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C100" t="s" s="5">
-        <v>310</v>
+        <v>108</v>
       </c>
       <c r="D100" t="s" s="5">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E100" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F100" s="6">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="G100" t="s" s="5">
         <v>16</v>
@@ -4437,29 +4656,937 @@
         <v>312</v>
       </c>
       <c r="C101" t="s" s="5">
-        <v>222</v>
+        <v>313</v>
       </c>
       <c r="D101" t="s" s="5">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E101" t="s" s="5">
         <v>11</v>
       </c>
       <c r="F101" s="6">
+        <v>180</v>
+      </c>
+      <c r="G101" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="102" ht="18.35" customHeight="1">
+      <c r="A102" t="s" s="5">
+        <v>314</v>
+      </c>
+      <c r="B102" t="s" s="5">
+        <v>315</v>
+      </c>
+      <c r="C102" t="s" s="5">
+        <v>225</v>
+      </c>
+      <c r="D102" t="s" s="5">
+        <v>47</v>
+      </c>
+      <c r="E102" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F102" s="6">
         <v>175</v>
       </c>
-      <c r="G101" t="s" s="5">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="102" ht="20.05" customHeight="1">
-      <c r="A102" s="7"/>
-      <c r="B102" s="7"/>
-      <c r="C102" s="7"/>
-      <c r="D102" s="7"/>
-      <c r="E102" s="7"/>
-      <c r="F102" s="7"/>
-      <c r="G102" s="7"/>
+      <c r="G102" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="103" ht="24.35" customHeight="1">
+      <c r="A103" t="s" s="7">
+        <v>316</v>
+      </c>
+      <c r="B103" t="s" s="7">
+        <v>317</v>
+      </c>
+      <c r="C103" t="s" s="7">
+        <v>318</v>
+      </c>
+      <c r="D103" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E103" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F103" s="8">
+        <v>175</v>
+      </c>
+      <c r="G103" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="104" ht="24.35" customHeight="1">
+      <c r="A104" t="s" s="7">
+        <v>319</v>
+      </c>
+      <c r="B104" t="s" s="7">
+        <v>320</v>
+      </c>
+      <c r="C104" t="s" s="7">
+        <v>321</v>
+      </c>
+      <c r="D104" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E104" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F104" s="8">
+        <v>178</v>
+      </c>
+      <c r="G104" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="105" ht="24.35" customHeight="1">
+      <c r="A105" t="s" s="7">
+        <v>322</v>
+      </c>
+      <c r="B105" t="s" s="7">
+        <v>323</v>
+      </c>
+      <c r="C105" t="s" s="7">
+        <v>324</v>
+      </c>
+      <c r="D105" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E105" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F105" s="8">
+        <v>174</v>
+      </c>
+      <c r="G105" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="106" ht="24.35" customHeight="1">
+      <c r="A106" t="s" s="7">
+        <v>325</v>
+      </c>
+      <c r="B106" t="s" s="7">
+        <v>326</v>
+      </c>
+      <c r="C106" t="s" s="7">
+        <v>327</v>
+      </c>
+      <c r="D106" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E106" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F106" s="8">
+        <v>177</v>
+      </c>
+      <c r="G106" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="107" ht="24.35" customHeight="1">
+      <c r="A107" t="s" s="7">
+        <v>328</v>
+      </c>
+      <c r="B107" t="s" s="7">
+        <v>329</v>
+      </c>
+      <c r="C107" t="s" s="7">
+        <v>330</v>
+      </c>
+      <c r="D107" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E107" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F107" s="8">
+        <v>172</v>
+      </c>
+      <c r="G107" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="108" ht="24.35" customHeight="1">
+      <c r="A108" t="s" s="7">
+        <v>331</v>
+      </c>
+      <c r="B108" t="s" s="7">
+        <v>332</v>
+      </c>
+      <c r="C108" t="s" s="7">
+        <v>333</v>
+      </c>
+      <c r="D108" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E108" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F108" s="8">
+        <v>187</v>
+      </c>
+      <c r="G108" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="109" ht="24.35" customHeight="1">
+      <c r="A109" t="s" s="7">
+        <v>334</v>
+      </c>
+      <c r="B109" t="s" s="7">
+        <v>335</v>
+      </c>
+      <c r="C109" t="s" s="7">
+        <v>194</v>
+      </c>
+      <c r="D109" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E109" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F109" s="8">
+        <v>168</v>
+      </c>
+      <c r="G109" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="110" ht="24.35" customHeight="1">
+      <c r="A110" t="s" s="7">
+        <v>336</v>
+      </c>
+      <c r="B110" t="s" s="7">
+        <v>337</v>
+      </c>
+      <c r="C110" t="s" s="7">
+        <v>338</v>
+      </c>
+      <c r="D110" t="s" s="7">
+        <v>339</v>
+      </c>
+      <c r="E110" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F110" s="8">
+        <v>168</v>
+      </c>
+      <c r="G110" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="111" ht="24.35" customHeight="1">
+      <c r="A111" t="s" s="7">
+        <v>340</v>
+      </c>
+      <c r="B111" t="s" s="7">
+        <v>341</v>
+      </c>
+      <c r="C111" t="s" s="7">
+        <v>342</v>
+      </c>
+      <c r="D111" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E111" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F111" s="8">
+        <v>170</v>
+      </c>
+      <c r="G111" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="112" ht="24.35" customHeight="1">
+      <c r="A112" t="s" s="7">
+        <v>343</v>
+      </c>
+      <c r="B112" t="s" s="7">
+        <v>344</v>
+      </c>
+      <c r="C112" t="s" s="7">
+        <v>117</v>
+      </c>
+      <c r="D112" t="s" s="7">
+        <v>345</v>
+      </c>
+      <c r="E112" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F112" s="8">
+        <v>168</v>
+      </c>
+      <c r="G112" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="113" ht="24.35" customHeight="1">
+      <c r="A113" t="s" s="7">
+        <v>346</v>
+      </c>
+      <c r="B113" t="s" s="7">
+        <v>347</v>
+      </c>
+      <c r="C113" t="s" s="7">
+        <v>348</v>
+      </c>
+      <c r="D113" t="s" s="7">
+        <v>345</v>
+      </c>
+      <c r="E113" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F113" s="8">
+        <v>182</v>
+      </c>
+      <c r="G113" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="114" ht="24.35" customHeight="1">
+      <c r="A114" t="s" s="7">
+        <v>349</v>
+      </c>
+      <c r="B114" t="s" s="7">
+        <v>350</v>
+      </c>
+      <c r="C114" t="s" s="7">
+        <v>276</v>
+      </c>
+      <c r="D114" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E114" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F114" s="8">
+        <v>173</v>
+      </c>
+      <c r="G114" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="115" ht="24.35" customHeight="1">
+      <c r="A115" t="s" s="7">
+        <v>351</v>
+      </c>
+      <c r="B115" t="s" s="7">
+        <v>352</v>
+      </c>
+      <c r="C115" t="s" s="7">
+        <v>353</v>
+      </c>
+      <c r="D115" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E115" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F115" s="8">
+        <v>175</v>
+      </c>
+      <c r="G115" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="116" ht="24.35" customHeight="1">
+      <c r="A116" t="s" s="7">
+        <v>354</v>
+      </c>
+      <c r="B116" t="s" s="7">
+        <v>355</v>
+      </c>
+      <c r="C116" t="s" s="7">
+        <v>356</v>
+      </c>
+      <c r="D116" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E116" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F116" s="8">
+        <v>164</v>
+      </c>
+      <c r="G116" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="117" ht="24.35" customHeight="1">
+      <c r="A117" t="s" s="7">
+        <v>357</v>
+      </c>
+      <c r="B117" t="s" s="7">
+        <v>358</v>
+      </c>
+      <c r="C117" t="s" s="7">
+        <v>359</v>
+      </c>
+      <c r="D117" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E117" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F117" s="8">
+        <v>176</v>
+      </c>
+      <c r="G117" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" ht="24.35" customHeight="1">
+      <c r="A118" t="s" s="7">
+        <v>360</v>
+      </c>
+      <c r="B118" t="s" s="7">
+        <v>361</v>
+      </c>
+      <c r="C118" t="s" s="7">
+        <v>300</v>
+      </c>
+      <c r="D118" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E118" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F118" s="8">
+        <v>190</v>
+      </c>
+      <c r="G118" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="119" ht="24.35" customHeight="1">
+      <c r="A119" t="s" s="7">
+        <v>362</v>
+      </c>
+      <c r="B119" t="s" s="7">
+        <v>363</v>
+      </c>
+      <c r="C119" t="s" s="7">
+        <v>128</v>
+      </c>
+      <c r="D119" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E119" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F119" s="8">
+        <v>179</v>
+      </c>
+      <c r="G119" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="120" ht="24.35" customHeight="1">
+      <c r="A120" t="s" s="7">
+        <v>364</v>
+      </c>
+      <c r="B120" t="s" s="7">
+        <v>365</v>
+      </c>
+      <c r="C120" t="s" s="7">
+        <v>366</v>
+      </c>
+      <c r="D120" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E120" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F120" s="8">
+        <v>179</v>
+      </c>
+      <c r="G120" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="121" ht="24.35" customHeight="1">
+      <c r="A121" t="s" s="7">
+        <v>367</v>
+      </c>
+      <c r="B121" t="s" s="7">
+        <v>368</v>
+      </c>
+      <c r="C121" t="s" s="7">
+        <v>369</v>
+      </c>
+      <c r="D121" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E121" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F121" s="8">
+        <v>230</v>
+      </c>
+      <c r="G121" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="122" ht="24.35" customHeight="1">
+      <c r="A122" t="s" s="7">
+        <v>370</v>
+      </c>
+      <c r="B122" t="s" s="7">
+        <v>371</v>
+      </c>
+      <c r="C122" t="s" s="7">
+        <v>372</v>
+      </c>
+      <c r="D122" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E122" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F122" s="8">
+        <v>155</v>
+      </c>
+      <c r="G122" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="123" ht="24.35" customHeight="1">
+      <c r="A123" t="s" s="7">
+        <v>373</v>
+      </c>
+      <c r="B123" t="s" s="7">
+        <v>374</v>
+      </c>
+      <c r="C123" t="s" s="7">
+        <v>324</v>
+      </c>
+      <c r="D123" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E123" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F123" s="8">
+        <v>183</v>
+      </c>
+      <c r="G123" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="124" ht="24.35" customHeight="1">
+      <c r="A124" t="s" s="7">
+        <v>375</v>
+      </c>
+      <c r="B124" t="s" s="7">
+        <v>376</v>
+      </c>
+      <c r="C124" t="s" s="7">
+        <v>203</v>
+      </c>
+      <c r="D124" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E124" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F124" s="8">
+        <v>168</v>
+      </c>
+      <c r="G124" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="125" ht="24.35" customHeight="1">
+      <c r="A125" t="s" s="7">
+        <v>377</v>
+      </c>
+      <c r="B125" t="s" s="7">
+        <v>378</v>
+      </c>
+      <c r="C125" t="s" s="7">
+        <v>379</v>
+      </c>
+      <c r="D125" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="E125" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F125" s="8">
+        <v>213</v>
+      </c>
+      <c r="G125" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="126" ht="24.35" customHeight="1">
+      <c r="A126" t="s" s="7">
+        <v>380</v>
+      </c>
+      <c r="B126" t="s" s="7">
+        <v>381</v>
+      </c>
+      <c r="C126" t="s" s="7">
+        <v>382</v>
+      </c>
+      <c r="D126" t="s" s="7">
+        <v>383</v>
+      </c>
+      <c r="E126" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="F126" s="8">
+        <v>168</v>
+      </c>
+      <c r="G126" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="127" ht="20.05" customHeight="1">
+      <c r="A127" s="9"/>
+      <c r="B127" s="9"/>
+      <c r="C127" s="9"/>
+      <c r="D127" s="9"/>
+      <c r="E127" s="9"/>
+      <c r="F127" s="9"/>
+      <c r="G127" s="9"/>
+    </row>
+    <row r="128" ht="20.05" customHeight="1">
+      <c r="A128" s="9"/>
+      <c r="B128" s="9"/>
+      <c r="C128" s="9"/>
+      <c r="D128" s="9"/>
+      <c r="E128" s="9"/>
+      <c r="F128" s="9"/>
+      <c r="G128" s="9"/>
+    </row>
+    <row r="129" ht="20.05" customHeight="1">
+      <c r="A129" s="9"/>
+      <c r="B129" s="9"/>
+      <c r="C129" s="9"/>
+      <c r="D129" s="9"/>
+      <c r="E129" s="9"/>
+      <c r="F129" s="9"/>
+      <c r="G129" s="9"/>
+    </row>
+    <row r="130" ht="20.05" customHeight="1">
+      <c r="A130" s="9"/>
+      <c r="B130" s="9"/>
+      <c r="C130" s="9"/>
+      <c r="D130" s="9"/>
+      <c r="E130" s="9"/>
+      <c r="F130" s="9"/>
+      <c r="G130" s="9"/>
+    </row>
+    <row r="131" ht="20.05" customHeight="1">
+      <c r="A131" s="9"/>
+      <c r="B131" s="9"/>
+      <c r="C131" s="9"/>
+      <c r="D131" s="9"/>
+      <c r="E131" s="9"/>
+      <c r="F131" s="9"/>
+      <c r="G131" s="9"/>
+    </row>
+    <row r="132" ht="20.05" customHeight="1">
+      <c r="A132" s="9"/>
+      <c r="B132" s="9"/>
+      <c r="C132" s="9"/>
+      <c r="D132" s="9"/>
+      <c r="E132" s="9"/>
+      <c r="F132" s="9"/>
+      <c r="G132" s="9"/>
+    </row>
+    <row r="133" ht="20.05" customHeight="1">
+      <c r="A133" s="9"/>
+      <c r="B133" s="9"/>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="F133" s="9"/>
+      <c r="G133" s="9"/>
+    </row>
+    <row r="134" ht="20.05" customHeight="1">
+      <c r="A134" s="9"/>
+      <c r="B134" s="9"/>
+      <c r="C134" s="9"/>
+      <c r="D134" s="9"/>
+      <c r="E134" s="9"/>
+      <c r="F134" s="9"/>
+      <c r="G134" s="9"/>
+    </row>
+    <row r="135" ht="20.05" customHeight="1">
+      <c r="A135" s="9"/>
+      <c r="B135" s="9"/>
+      <c r="C135" s="9"/>
+      <c r="D135" s="9"/>
+      <c r="E135" s="9"/>
+      <c r="F135" s="9"/>
+      <c r="G135" s="9"/>
+    </row>
+    <row r="136" ht="20.05" customHeight="1">
+      <c r="A136" s="9"/>
+      <c r="B136" s="9"/>
+      <c r="C136" s="9"/>
+      <c r="D136" s="9"/>
+      <c r="E136" s="9"/>
+      <c r="F136" s="9"/>
+      <c r="G136" s="9"/>
+    </row>
+    <row r="137" ht="20.05" customHeight="1">
+      <c r="A137" s="9"/>
+      <c r="B137" s="9"/>
+      <c r="C137" s="9"/>
+      <c r="D137" s="9"/>
+      <c r="E137" s="9"/>
+      <c r="F137" s="9"/>
+      <c r="G137" s="9"/>
+    </row>
+    <row r="138" ht="20.05" customHeight="1">
+      <c r="A138" s="9"/>
+      <c r="B138" s="9"/>
+      <c r="C138" s="9"/>
+      <c r="D138" s="9"/>
+      <c r="E138" s="9"/>
+      <c r="F138" s="9"/>
+      <c r="G138" s="9"/>
+    </row>
+    <row r="139" ht="20.05" customHeight="1">
+      <c r="A139" s="9"/>
+      <c r="B139" s="9"/>
+      <c r="C139" s="9"/>
+      <c r="D139" s="9"/>
+      <c r="E139" s="9"/>
+      <c r="F139" s="9"/>
+      <c r="G139" s="9"/>
+    </row>
+    <row r="140" ht="20.05" customHeight="1">
+      <c r="A140" s="9"/>
+      <c r="B140" s="9"/>
+      <c r="C140" s="9"/>
+      <c r="D140" s="9"/>
+      <c r="E140" s="9"/>
+      <c r="F140" s="9"/>
+      <c r="G140" s="9"/>
+    </row>
+    <row r="141" ht="20.05" customHeight="1">
+      <c r="A141" s="9"/>
+      <c r="B141" s="9"/>
+      <c r="C141" s="9"/>
+      <c r="D141" s="9"/>
+      <c r="E141" s="9"/>
+      <c r="F141" s="9"/>
+      <c r="G141" s="9"/>
+    </row>
+    <row r="142" ht="20.05" customHeight="1">
+      <c r="A142" s="9"/>
+      <c r="B142" s="9"/>
+      <c r="C142" s="9"/>
+      <c r="D142" s="9"/>
+      <c r="E142" s="9"/>
+      <c r="F142" s="9"/>
+      <c r="G142" s="9"/>
+    </row>
+    <row r="143" ht="20.05" customHeight="1">
+      <c r="A143" s="9"/>
+      <c r="B143" s="9"/>
+      <c r="C143" s="9"/>
+      <c r="D143" s="9"/>
+      <c r="E143" s="9"/>
+      <c r="F143" s="9"/>
+      <c r="G143" s="9"/>
+    </row>
+    <row r="144" ht="20.05" customHeight="1">
+      <c r="A144" s="9"/>
+      <c r="B144" s="9"/>
+      <c r="C144" s="9"/>
+      <c r="D144" s="9"/>
+      <c r="E144" s="9"/>
+      <c r="F144" s="9"/>
+      <c r="G144" s="9"/>
+    </row>
+    <row r="145" ht="20.05" customHeight="1">
+      <c r="A145" s="9"/>
+      <c r="B145" s="9"/>
+      <c r="C145" s="9"/>
+      <c r="D145" s="9"/>
+      <c r="E145" s="9"/>
+      <c r="F145" s="9"/>
+      <c r="G145" s="9"/>
+    </row>
+    <row r="146" ht="20.05" customHeight="1">
+      <c r="A146" s="9"/>
+      <c r="B146" s="9"/>
+      <c r="C146" s="9"/>
+      <c r="D146" s="9"/>
+      <c r="E146" s="9"/>
+      <c r="F146" s="9"/>
+      <c r="G146" s="9"/>
+    </row>
+    <row r="147" ht="20.05" customHeight="1">
+      <c r="A147" s="9"/>
+      <c r="B147" s="9"/>
+      <c r="C147" s="9"/>
+      <c r="D147" s="9"/>
+      <c r="E147" s="9"/>
+      <c r="F147" s="9"/>
+      <c r="G147" s="9"/>
+    </row>
+    <row r="148" ht="20.05" customHeight="1">
+      <c r="A148" s="9"/>
+      <c r="B148" s="9"/>
+      <c r="C148" s="9"/>
+      <c r="D148" s="9"/>
+      <c r="E148" s="9"/>
+      <c r="F148" s="9"/>
+      <c r="G148" s="9"/>
+    </row>
+    <row r="149" ht="20.05" customHeight="1">
+      <c r="A149" s="9"/>
+      <c r="B149" s="9"/>
+      <c r="C149" s="9"/>
+      <c r="D149" s="9"/>
+      <c r="E149" s="9"/>
+      <c r="F149" s="9"/>
+      <c r="G149" s="9"/>
+    </row>
+    <row r="150" ht="20.05" customHeight="1">
+      <c r="A150" s="9"/>
+      <c r="B150" s="9"/>
+      <c r="C150" s="9"/>
+      <c r="D150" s="9"/>
+      <c r="E150" s="9"/>
+      <c r="F150" s="9"/>
+      <c r="G150" s="9"/>
+    </row>
+    <row r="151" ht="20.05" customHeight="1">
+      <c r="A151" s="9"/>
+      <c r="B151" s="9"/>
+      <c r="C151" s="9"/>
+      <c r="D151" s="9"/>
+      <c r="E151" s="9"/>
+      <c r="F151" s="9"/>
+      <c r="G151" s="9"/>
+    </row>
+    <row r="152" ht="20.05" customHeight="1">
+      <c r="A152" s="9"/>
+      <c r="B152" s="9"/>
+      <c r="C152" s="9"/>
+      <c r="D152" s="9"/>
+      <c r="E152" s="9"/>
+      <c r="F152" s="9"/>
+      <c r="G152" s="9"/>
+    </row>
+    <row r="153" ht="20.05" customHeight="1">
+      <c r="A153" s="9"/>
+      <c r="B153" s="9"/>
+      <c r="C153" s="9"/>
+      <c r="D153" s="9"/>
+      <c r="E153" s="9"/>
+      <c r="F153" s="9"/>
+      <c r="G153" s="9"/>
+    </row>
+    <row r="154" ht="20.05" customHeight="1">
+      <c r="A154" s="9"/>
+      <c r="B154" s="9"/>
+      <c r="C154" s="9"/>
+      <c r="D154" s="9"/>
+      <c r="E154" s="9"/>
+      <c r="F154" s="9"/>
+      <c r="G154" s="9"/>
+    </row>
+    <row r="155" ht="20.05" customHeight="1">
+      <c r="A155" s="9"/>
+      <c r="B155" s="9"/>
+      <c r="C155" s="9"/>
+      <c r="D155" s="9"/>
+      <c r="E155" s="9"/>
+      <c r="F155" s="9"/>
+      <c r="G155" s="9"/>
+    </row>
+    <row r="156" ht="20.05" customHeight="1">
+      <c r="A156" s="9"/>
+      <c r="B156" s="9"/>
+      <c r="C156" s="9"/>
+      <c r="D156" s="9"/>
+      <c r="E156" s="9"/>
+      <c r="F156" s="9"/>
+      <c r="G156" s="9"/>
+    </row>
+    <row r="157" ht="20.05" customHeight="1">
+      <c r="A157" s="9"/>
+      <c r="B157" s="9"/>
+      <c r="C157" s="9"/>
+      <c r="D157" s="9"/>
+      <c r="E157" s="9"/>
+      <c r="F157" s="9"/>
+      <c r="G157" s="9"/>
+    </row>
+    <row r="158" ht="20.05" customHeight="1">
+      <c r="A158" s="9"/>
+      <c r="B158" s="9"/>
+      <c r="C158" s="9"/>
+      <c r="D158" s="9"/>
+      <c r="E158" s="9"/>
+      <c r="F158" s="9"/>
+      <c r="G158" s="9"/>
+    </row>
+    <row r="159" ht="20.05" customHeight="1">
+      <c r="A159" s="9"/>
+      <c r="B159" s="9"/>
+      <c r="C159" s="9"/>
+      <c r="D159" s="9"/>
+      <c r="E159" s="9"/>
+      <c r="F159" s="9"/>
+      <c r="G159" s="9"/>
+    </row>
+    <row r="160" ht="20.05" customHeight="1">
+      <c r="A160" s="9"/>
+      <c r="B160" s="9"/>
+      <c r="C160" s="9"/>
+      <c r="D160" s="9"/>
+      <c r="E160" s="9"/>
+      <c r="F160" s="9"/>
+      <c r="G160" s="9"/>
+    </row>
+    <row r="161" ht="20.05" customHeight="1">
+      <c r="A161" s="9"/>
+      <c r="B161" s="9"/>
+      <c r="C161" s="9"/>
+      <c r="D161" s="9"/>
+      <c r="E161" s="9"/>
+      <c r="F161" s="9"/>
+      <c r="G161" s="9"/>
+    </row>
+    <row r="162" ht="20.05" customHeight="1">
+      <c r="A162" s="9"/>
+      <c r="B162" s="9"/>
+      <c r="C162" s="9"/>
+      <c r="D162" s="9"/>
+      <c r="E162" s="9"/>
+      <c r="F162" s="9"/>
+      <c r="G162" s="9"/>
+    </row>
+    <row r="163" ht="20.05" customHeight="1">
+      <c r="A163" s="9"/>
+      <c r="B163" s="9"/>
+      <c r="C163" s="9"/>
+      <c r="D163" s="9"/>
+      <c r="E163" s="9"/>
+      <c r="F163" s="9"/>
+      <c r="G163" s="9"/>
+    </row>
+    <row r="164" ht="20.05" customHeight="1">
+      <c r="A164" s="9"/>
+      <c r="B164" s="9"/>
+      <c r="C164" s="9"/>
+      <c r="D164" s="9"/>
+      <c r="E164" s="9"/>
+      <c r="F164" s="9"/>
+      <c r="G164" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>